<commit_message>
PPT: OE4 criterios, sin tabu | H.U. ordenados por prioridad
</commit_message>
<xml_diff>
--- a/Documentación/Análisis/Lista de Requerimientos - Historias de Usuarios.xlsx
+++ b/Documentación/Análisis/Lista de Requerimientos - Historias de Usuarios.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="20115" windowHeight="7995" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="20115" windowHeight="7995" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Control de versiones" sheetId="8" r:id="rId1"/>
@@ -17,7 +17,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Historias de Usuarios'!$C$1:$J$58</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -1367,8 +1366,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1704,7 +1703,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1778,7 +1777,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1813,7 +1811,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1989,14 +1986,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="10" style="13"/>
     <col min="3" max="3" width="11.28515625" style="13" customWidth="1"/>
@@ -2006,7 +2003,7 @@
     <col min="7" max="16384" width="10" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" s="12"/>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -2016,7 +2013,7 @@
       <c r="G1" s="12"/>
       <c r="H1" s="12"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" s="12"/>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
@@ -2026,7 +2023,7 @@
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3" s="15"/>
       <c r="B3" s="31" t="s">
         <v>106</v>
@@ -2038,7 +2035,7 @@
       <c r="G3" s="16"/>
       <c r="H3" s="12"/>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="15" customHeight="1">
       <c r="A4" s="15"/>
       <c r="B4" s="17" t="s">
         <v>107</v>
@@ -2058,7 +2055,7 @@
       <c r="G4" s="18"/>
       <c r="H4" s="12"/>
     </row>
-    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="15">
       <c r="A5" s="15"/>
       <c r="B5" s="19">
         <v>1</v>
@@ -2078,7 +2075,7 @@
       <c r="G5" s="18"/>
       <c r="H5" s="12"/>
     </row>
-    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="15">
       <c r="A6" s="12"/>
       <c r="B6" s="19">
         <v>2</v>
@@ -2098,7 +2095,7 @@
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
     </row>
-    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="15">
       <c r="A7" s="12"/>
       <c r="B7" s="19">
         <v>3</v>
@@ -2118,7 +2115,7 @@
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -2128,7 +2125,7 @@
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
@@ -2138,7 +2135,7 @@
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
@@ -2148,7 +2145,7 @@
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8">
       <c r="A11" s="12"/>
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
@@ -2158,7 +2155,7 @@
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8">
       <c r="A12" s="12"/>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
@@ -2168,7 +2165,7 @@
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8">
       <c r="A13" s="12"/>
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
@@ -2187,14 +2184,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C1:J58"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2.7109375" style="21" customWidth="1"/>
     <col min="2" max="2" width="2.5703125" style="21" customWidth="1"/>
@@ -2208,7 +2205,7 @@
     <col min="11" max="16384" width="11.42578125" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:10" ht="30" customHeight="1">
       <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2234,99 +2231,99 @@
         <v>318</v>
       </c>
     </row>
-    <row r="2" spans="3:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:10" ht="45">
       <c r="C2" s="25" t="s">
-        <v>116</v>
+        <v>266</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="E2" s="29" t="s">
         <v>117</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>120</v>
+        <v>332</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>124</v>
+        <v>338</v>
       </c>
       <c r="H2" s="27">
         <v>3</v>
       </c>
       <c r="I2" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="3:10" ht="105" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="3:10" ht="45">
       <c r="C3" s="25" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="E3" s="29" t="s">
         <v>117</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>121</v>
+        <v>333</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>123</v>
+        <v>337</v>
       </c>
       <c r="H3" s="27">
         <v>3</v>
       </c>
       <c r="I3" s="25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="3:10" ht="75" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="3:10" ht="45">
       <c r="C4" s="25" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>354</v>
+        <v>141</v>
       </c>
       <c r="E4" s="29" t="s">
         <v>117</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>125</v>
+        <v>139</v>
       </c>
       <c r="G4" s="24" t="s">
-        <v>339</v>
+        <v>140</v>
       </c>
       <c r="H4" s="25">
         <v>3</v>
       </c>
       <c r="I4" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="3:10" ht="45" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" ht="45">
       <c r="C5" s="25" t="s">
-        <v>266</v>
+        <v>281</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>332</v>
+        <v>139</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>338</v>
+        <v>140</v>
       </c>
       <c r="H5" s="25">
         <v>3</v>
@@ -2335,24 +2332,24 @@
         <v>1</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="3:10" ht="45" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" ht="30">
       <c r="C6" s="25" t="s">
-        <v>267</v>
+        <v>296</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>127</v>
+        <v>192</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>117</v>
+        <v>326</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>333</v>
+        <v>190</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>337</v>
+        <v>191</v>
       </c>
       <c r="H6" s="25">
         <v>3</v>
@@ -2361,336 +2358,336 @@
         <v>1</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="3:10" ht="60" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" ht="75">
       <c r="C7" s="25" t="s">
-        <v>268</v>
+        <v>297</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>128</v>
+        <v>194</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>117</v>
+        <v>326</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>335</v>
+        <v>195</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>336</v>
+        <v>193</v>
       </c>
       <c r="H7" s="25">
         <v>3</v>
       </c>
       <c r="I7" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="3:10" ht="60" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10" ht="75">
       <c r="C8" s="25" t="s">
-        <v>269</v>
+        <v>298</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>130</v>
+        <v>198</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>117</v>
+        <v>326</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>129</v>
+        <v>196</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>149</v>
+        <v>197</v>
       </c>
       <c r="H8" s="25">
         <v>3</v>
       </c>
       <c r="I8" s="25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="3:10" ht="75" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" ht="60">
       <c r="C9" s="25" t="s">
-        <v>270</v>
+        <v>303</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>132</v>
+        <v>263</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>117</v>
+        <v>326</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>133</v>
+        <v>210</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>131</v>
+        <v>211</v>
       </c>
       <c r="H9" s="25">
         <v>3</v>
       </c>
       <c r="I9" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="3:10" ht="75" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" ht="60">
       <c r="C10" s="25" t="s">
-        <v>271</v>
+        <v>309</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>319</v>
+        <v>225</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>117</v>
+        <v>326</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>142</v>
+        <v>224</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>134</v>
+        <v>228</v>
       </c>
       <c r="H10" s="25">
         <v>3</v>
       </c>
       <c r="I10" s="25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="3:10" ht="45" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" ht="60">
       <c r="C11" s="25" t="s">
-        <v>272</v>
+        <v>116</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="E11" s="29" t="s">
         <v>117</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="H11" s="25">
         <v>3</v>
       </c>
       <c r="I11" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="3:10" ht="75" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" ht="75">
       <c r="C12" s="25" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>171</v>
+        <v>354</v>
       </c>
       <c r="E12" s="29" t="s">
         <v>117</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>169</v>
+        <v>125</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>170</v>
+        <v>339</v>
       </c>
       <c r="H12" s="25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I12" s="25">
+        <v>2</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10" ht="60">
+      <c r="C13" s="25" t="s">
+        <v>268</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="H13" s="25">
         <v>3</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="3:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="C13" s="25" t="s">
-        <v>274</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="E13" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="H13" s="25">
-        <v>1</v>
       </c>
       <c r="I13" s="25">
         <v>2</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="3:10" ht="45" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10" ht="75">
       <c r="C14" s="25" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>343</v>
+        <v>132</v>
       </c>
       <c r="E14" s="29" t="s">
-        <v>10</v>
+        <v>117</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>341</v>
+        <v>133</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>342</v>
+        <v>131</v>
       </c>
       <c r="H14" s="25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I14" s="25">
         <v>2</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="3:10" ht="45" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="3:10" ht="45">
       <c r="C15" s="25" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>138</v>
+        <v>154</v>
       </c>
       <c r="E15" s="29" t="s">
         <v>10</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>136</v>
+        <v>153</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>137</v>
+        <v>155</v>
       </c>
       <c r="H15" s="25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I15" s="25">
         <v>2</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="3:10" ht="90" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="3:10" ht="75">
       <c r="C16" s="25" t="s">
-        <v>277</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>146</v>
+        <v>295</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>256</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>10</v>
+        <v>326</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>144</v>
+        <v>254</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>145</v>
+        <v>255</v>
       </c>
       <c r="H16" s="25">
         <v>3</v>
       </c>
       <c r="I16" s="25">
+        <v>2</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10" ht="60">
+      <c r="C17" s="25" t="s">
+        <v>305</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>326</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="H17" s="25">
         <v>3</v>
       </c>
-      <c r="J16" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="3:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="C17" s="25" t="s">
-        <v>278</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="E17" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="H17" s="25">
-        <v>1</v>
-      </c>
       <c r="I17" s="25">
+        <v>2</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10" ht="60">
+      <c r="C18" s="25" t="s">
+        <v>307</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="E18" s="29" t="s">
+        <v>326</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="H18" s="25">
         <v>3</v>
       </c>
-      <c r="J17" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="3:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="C18" s="25" t="s">
-        <v>279</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>323</v>
-      </c>
-      <c r="E18" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="H18" s="25">
-        <v>1</v>
-      </c>
       <c r="I18" s="25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="3:10" ht="45" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="3:10" ht="75">
       <c r="C19" s="25" t="s">
-        <v>280</v>
+        <v>308</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>154</v>
+        <v>223</v>
       </c>
       <c r="E19" s="29" t="s">
-        <v>10</v>
+        <v>326</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>153</v>
+        <v>222</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>155</v>
+        <v>227</v>
       </c>
       <c r="H19" s="25">
         <v>3</v>
@@ -2699,192 +2696,192 @@
         <v>2</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="3:10" ht="45" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="3:10" ht="105">
       <c r="C20" s="25" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>156</v>
+        <v>122</v>
       </c>
       <c r="E20" s="29" t="s">
-        <v>10</v>
+        <v>117</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="H20" s="25">
         <v>3</v>
       </c>
       <c r="I20" s="25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="3:10" ht="45" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="3:10" ht="60">
       <c r="C21" s="25" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>159</v>
+        <v>130</v>
       </c>
       <c r="E21" s="29" t="s">
-        <v>10</v>
+        <v>117</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>157</v>
+        <v>129</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="H21" s="25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I21" s="25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="3:10" ht="60" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="3:10" ht="75">
       <c r="C22" s="25" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>161</v>
+        <v>319</v>
       </c>
       <c r="E22" s="29" t="s">
-        <v>10</v>
+        <v>117</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>329</v>
+        <v>134</v>
       </c>
       <c r="H22" s="25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I22" s="25">
         <v>3</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="3:10" ht="60" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="3:10" ht="90">
       <c r="C23" s="25" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>320</v>
+        <v>146</v>
       </c>
       <c r="E23" s="29" t="s">
         <v>10</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="H23" s="25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I23" s="25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="3:10" ht="75" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="3:10" ht="45">
       <c r="C24" s="25" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>321</v>
+        <v>174</v>
       </c>
       <c r="E24" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="H24" s="25">
+        <v>3</v>
+      </c>
+      <c r="I24" s="25">
+        <v>3</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="3:10" ht="60">
+      <c r="C25" s="25" t="s">
+        <v>311</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>410</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>326</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="H25" s="25">
+        <v>3</v>
+      </c>
+      <c r="I25" s="25">
+        <v>3</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="3:10" ht="45">
+      <c r="C26" s="25" t="s">
+        <v>276</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E26" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="F24" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="H24" s="25">
-        <v>1</v>
-      </c>
-      <c r="I24" s="25">
-        <v>1</v>
-      </c>
-      <c r="J24" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="3:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="C25" s="25" t="s">
-        <v>286</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="E25" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="H25" s="25">
-        <v>1</v>
-      </c>
-      <c r="I25" s="25">
+      <c r="F26" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="H26" s="25">
         <v>2</v>
       </c>
-      <c r="J25" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="26" spans="3:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="C26" s="25" t="s">
-        <v>287</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="E26" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="H26" s="25">
-        <v>3</v>
-      </c>
       <c r="I26" s="25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="27" spans="3:10" ht="60" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="3:10" ht="60">
       <c r="C27" s="25" t="s">
         <v>288</v>
       </c>
@@ -2910,7 +2907,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="3:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:10" ht="75">
       <c r="C28" s="25" t="s">
         <v>289</v>
       </c>
@@ -2936,7 +2933,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="3:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:10" ht="45">
       <c r="C29" s="25" t="s">
         <v>290</v>
       </c>
@@ -2962,47 +2959,47 @@
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="3:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:10" ht="30">
       <c r="C30" s="25" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>181</v>
+        <v>328</v>
       </c>
       <c r="E30" s="29" t="s">
         <v>118</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>180</v>
+        <v>258</v>
       </c>
       <c r="H30" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I30" s="25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="31" spans="3:10" ht="30" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="3:10" ht="75">
       <c r="C31" s="25" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>328</v>
+        <v>201</v>
       </c>
       <c r="E31" s="29" t="s">
-        <v>118</v>
+        <v>326</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>258</v>
+        <v>200</v>
       </c>
       <c r="H31" s="25">
         <v>2</v>
@@ -3011,180 +3008,180 @@
         <v>2</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="32" spans="3:10" ht="90" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="3:10" ht="60">
       <c r="C32" s="25" t="s">
-        <v>293</v>
+        <v>304</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>189</v>
+        <v>262</v>
       </c>
       <c r="E32" s="29" t="s">
-        <v>118</v>
+        <v>326</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>187</v>
+        <v>212</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="H32" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I32" s="25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J32" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="33" spans="3:10" ht="60" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="3:10" ht="45">
       <c r="C33" s="25" t="s">
-        <v>294</v>
+        <v>312</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
       <c r="E33" s="29" t="s">
-        <v>118</v>
+        <v>326</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>249</v>
+        <v>364</v>
       </c>
       <c r="H33" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I33" s="25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J33" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="34" spans="3:10" ht="75" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="3:10" ht="45">
       <c r="C34" s="25" t="s">
-        <v>295</v>
-      </c>
-      <c r="D34" s="22" t="s">
-        <v>256</v>
+        <v>313</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>240</v>
       </c>
       <c r="E34" s="29" t="s">
-        <v>326</v>
+        <v>10</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>254</v>
+        <v>233</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="H34" s="25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I34" s="25">
         <v>2</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="35" spans="3:10" ht="30" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="35" spans="3:10" ht="45">
       <c r="C35" s="25" t="s">
-        <v>296</v>
+        <v>315</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>192</v>
+        <v>238</v>
       </c>
       <c r="E35" s="29" t="s">
-        <v>326</v>
+        <v>118</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>190</v>
+        <v>236</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>191</v>
+        <v>237</v>
       </c>
       <c r="H35" s="25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I35" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="36" spans="3:10" ht="75" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="36" spans="3:10" ht="45">
       <c r="C36" s="25" t="s">
-        <v>297</v>
+        <v>316</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>194</v>
+        <v>242</v>
       </c>
       <c r="E36" s="29" t="s">
-        <v>326</v>
+        <v>118</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>195</v>
+        <v>243</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>193</v>
+        <v>241</v>
       </c>
       <c r="H36" s="25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I36" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J36" s="7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="37" spans="3:10" ht="75" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="37" spans="3:10" ht="45">
       <c r="C37" s="25" t="s">
-        <v>298</v>
+        <v>317</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>198</v>
+        <v>246</v>
       </c>
       <c r="E37" s="29" t="s">
         <v>326</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>196</v>
+        <v>244</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>197</v>
+        <v>245</v>
       </c>
       <c r="H37" s="25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I37" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J37" s="7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="38" spans="3:10" ht="75" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="38" spans="3:10" ht="60">
       <c r="C38" s="25" t="s">
-        <v>299</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>201</v>
+        <v>344</v>
+      </c>
+      <c r="D38" s="22" t="s">
+        <v>368</v>
       </c>
       <c r="E38" s="29" t="s">
         <v>326</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>199</v>
+        <v>366</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>200</v>
+        <v>367</v>
       </c>
       <c r="H38" s="25">
         <v>2</v>
@@ -3193,180 +3190,180 @@
         <v>2</v>
       </c>
       <c r="J38" s="7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="39" spans="3:10" ht="75" x14ac:dyDescent="0.25">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="39" spans="3:10" ht="60">
       <c r="C39" s="25" t="s">
-        <v>300</v>
+        <v>283</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>204</v>
+        <v>161</v>
       </c>
       <c r="E39" s="29" t="s">
-        <v>326</v>
+        <v>10</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>202</v>
+        <v>160</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>203</v>
+        <v>329</v>
       </c>
       <c r="H39" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I39" s="25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J39" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="40" spans="3:10" ht="75" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="3:10" ht="45">
       <c r="C40" s="25" t="s">
-        <v>301</v>
+        <v>282</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>324</v>
+        <v>159</v>
       </c>
       <c r="E40" s="29" t="s">
-        <v>326</v>
+        <v>10</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>205</v>
+        <v>157</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>206</v>
+        <v>158</v>
       </c>
       <c r="H40" s="25">
         <v>1</v>
       </c>
       <c r="I40" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J40" s="7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="41" spans="3:10" ht="60" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="3:10" ht="60">
       <c r="C41" s="25" t="s">
-        <v>302</v>
+        <v>284</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E41" s="29" t="s">
-        <v>326</v>
+        <v>10</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>208</v>
+        <v>162</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>209</v>
+        <v>163</v>
       </c>
       <c r="H41" s="25">
         <v>1</v>
       </c>
       <c r="I41" s="25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J41" s="7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="42" spans="3:10" ht="60" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="3:10" ht="75">
       <c r="C42" s="25" t="s">
-        <v>303</v>
+        <v>285</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>263</v>
+        <v>321</v>
       </c>
       <c r="E42" s="29" t="s">
-        <v>326</v>
+        <v>10</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>210</v>
+        <v>165</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>211</v>
+        <v>166</v>
       </c>
       <c r="H42" s="25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I42" s="25">
         <v>1</v>
       </c>
       <c r="J42" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="43" spans="3:10" ht="60" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="3:10" ht="75">
       <c r="C43" s="25" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>262</v>
+        <v>204</v>
       </c>
       <c r="E43" s="29" t="s">
         <v>326</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="H43" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I43" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J43" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="44" spans="3:10" ht="60" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="44" spans="3:10" ht="30">
       <c r="C44" s="25" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="E44" s="29" t="s">
         <v>326</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="H44" s="25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I44" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J44" s="7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="45" spans="3:10" ht="30" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="3:10" ht="45">
       <c r="C45" s="25" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
       <c r="E45" s="29" t="s">
         <v>326</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>218</v>
+        <v>229</v>
       </c>
       <c r="H45" s="25">
         <v>1</v>
@@ -3375,206 +3372,206 @@
         <v>1</v>
       </c>
       <c r="J45" s="7" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="46" spans="3:10" ht="60" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="3:10" ht="75">
       <c r="C46" s="25" t="s">
-        <v>307</v>
+        <v>274</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>261</v>
+        <v>164</v>
       </c>
       <c r="E46" s="29" t="s">
-        <v>326</v>
+        <v>10</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>220</v>
+        <v>135</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>215</v>
+        <v>143</v>
       </c>
       <c r="H46" s="25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I46" s="25">
         <v>2</v>
       </c>
       <c r="J46" s="7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="47" spans="3:10" ht="75" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" spans="3:10" ht="45">
       <c r="C47" s="25" t="s">
-        <v>308</v>
+        <v>275</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>223</v>
+        <v>343</v>
       </c>
       <c r="E47" s="29" t="s">
-        <v>326</v>
+        <v>10</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>222</v>
+        <v>341</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>227</v>
+        <v>342</v>
       </c>
       <c r="H47" s="25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I47" s="25">
         <v>2</v>
       </c>
       <c r="J47" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="48" spans="3:10" ht="60" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="48" spans="3:10" ht="90">
       <c r="C48" s="25" t="s">
-        <v>309</v>
+        <v>286</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>225</v>
+        <v>355</v>
       </c>
       <c r="E48" s="29" t="s">
-        <v>326</v>
+        <v>10</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>224</v>
+        <v>167</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>228</v>
+        <v>168</v>
       </c>
       <c r="H48" s="25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I48" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J48" s="7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="49" spans="3:10" ht="45" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="49" spans="3:10" ht="75">
       <c r="C49" s="25" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>230</v>
+        <v>324</v>
       </c>
       <c r="E49" s="29" t="s">
         <v>326</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>226</v>
+        <v>205</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>229</v>
+        <v>206</v>
       </c>
       <c r="H49" s="25">
         <v>1</v>
       </c>
       <c r="I49" s="25">
+        <v>2</v>
+      </c>
+      <c r="J49" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="50" spans="3:10" ht="75">
+      <c r="C50" s="25" t="s">
+        <v>273</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E50" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="H50" s="25">
         <v>1</v>
-      </c>
-      <c r="J49" s="7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="50" spans="3:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="C50" s="25" t="s">
-        <v>311</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>410</v>
-      </c>
-      <c r="E50" s="29" t="s">
-        <v>326</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>411</v>
-      </c>
-      <c r="G50" s="5" t="s">
-        <v>412</v>
-      </c>
-      <c r="H50" s="25">
-        <v>3</v>
       </c>
       <c r="I50" s="25">
         <v>3</v>
       </c>
       <c r="J50" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="51" spans="3:10" ht="45" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51" spans="3:10" ht="105">
       <c r="C51" s="25" t="s">
-        <v>312</v>
+        <v>278</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>232</v>
+        <v>147</v>
       </c>
       <c r="E51" s="29" t="s">
-        <v>326</v>
+        <v>10</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>231</v>
+        <v>148</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>364</v>
+        <v>150</v>
       </c>
       <c r="H51" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I51" s="25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J51" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="52" spans="3:10" ht="45" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="52" spans="3:10" ht="45">
       <c r="C52" s="25" t="s">
-        <v>313</v>
+        <v>279</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>240</v>
+        <v>323</v>
       </c>
       <c r="E52" s="29" t="s">
         <v>10</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>233</v>
+        <v>151</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>234</v>
+        <v>152</v>
       </c>
       <c r="H52" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I52" s="25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J52" s="7" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="53" spans="3:10" ht="90" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="53" spans="3:10" ht="75">
       <c r="C53" s="25" t="s">
-        <v>314</v>
+        <v>291</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>239</v>
+        <v>181</v>
       </c>
       <c r="E53" s="29" t="s">
-        <v>10</v>
+        <v>118</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>235</v>
+        <v>179</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>365</v>
+        <v>180</v>
       </c>
       <c r="H53" s="25">
         <v>1</v>
@@ -3583,114 +3580,114 @@
         <v>3</v>
       </c>
       <c r="J53" s="7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="54" spans="3:10" ht="45" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="54" spans="3:10" ht="90">
       <c r="C54" s="25" t="s">
-        <v>315</v>
+        <v>293</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>238</v>
+        <v>189</v>
       </c>
       <c r="E54" s="29" t="s">
         <v>118</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>236</v>
+        <v>187</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>237</v>
+        <v>188</v>
       </c>
       <c r="H54" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I54" s="25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J54" s="7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="55" spans="3:10" ht="45" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="55" spans="3:10" ht="60">
       <c r="C55" s="25" t="s">
-        <v>316</v>
+        <v>294</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="E55" s="29" t="s">
         <v>118</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="H55" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I55" s="25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J55" s="7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="56" spans="3:10" ht="45" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="56" spans="3:10" ht="60">
       <c r="C56" s="25" t="s">
-        <v>317</v>
+        <v>302</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>246</v>
+        <v>322</v>
       </c>
       <c r="E56" s="29" t="s">
         <v>326</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>244</v>
+        <v>208</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>245</v>
+        <v>209</v>
       </c>
       <c r="H56" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I56" s="25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J56" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="57" spans="3:10" ht="60" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="57" spans="3:10" ht="90">
       <c r="C57" s="25" t="s">
-        <v>344</v>
-      </c>
-      <c r="D57" s="22" t="s">
-        <v>368</v>
+        <v>314</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>239</v>
       </c>
       <c r="E57" s="29" t="s">
-        <v>326</v>
+        <v>10</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>366</v>
+        <v>235</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="H57" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I57" s="25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J57" s="7" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="58" spans="3:10" ht="45" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="58" spans="3:10" ht="45">
       <c r="C58" s="25" t="s">
         <v>413</v>
       </c>
@@ -3718,20 +3715,24 @@
     </row>
   </sheetData>
   <autoFilter ref="C1:J58"/>
+  <sortState ref="C2:J58">
+    <sortCondition descending="1" ref="H2:H58"/>
+    <sortCondition ref="I2:I58"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C1:I58"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49:C58"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.42578125" style="8" customWidth="1"/>
     <col min="2" max="2" width="3.85546875" style="8" customWidth="1"/>
@@ -3744,7 +3745,7 @@
     <col min="10" max="16384" width="11.42578125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:9" ht="21.75" customHeight="1">
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3758,11 +3759,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="3:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:9" ht="45">
       <c r="C2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="22" t="s">
         <v>331</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -3779,11 +3780,11 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="3:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:9" ht="45">
       <c r="C3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="22" t="s">
         <v>56</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -3800,11 +3801,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:9" ht="30">
       <c r="C4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="22" t="s">
         <v>347</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -3821,11 +3822,11 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="3:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:9" ht="60">
       <c r="C5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="22" t="s">
         <v>348</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -3835,11 +3836,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="3:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:9" ht="45">
       <c r="C6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="22" t="s">
         <v>67</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -3849,7 +3850,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:9" ht="30">
       <c r="C7" s="7" t="s">
         <v>22</v>
       </c>
@@ -3863,11 +3864,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:9" ht="30">
       <c r="C8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="22" t="s">
         <v>48</v>
       </c>
       <c r="E8" s="2" t="s">
@@ -3877,11 +3878,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:9" ht="30">
       <c r="C9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="22" t="s">
         <v>49</v>
       </c>
       <c r="E9" s="2" t="s">
@@ -3891,11 +3892,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:9" ht="30">
       <c r="C10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="22" t="s">
         <v>50</v>
       </c>
       <c r="E10" s="2" t="s">
@@ -3905,11 +3906,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:9" ht="30">
       <c r="C11" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="22" t="s">
         <v>57</v>
       </c>
       <c r="E11" s="2" t="s">
@@ -3919,11 +3920,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="3:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:9" ht="45">
       <c r="C12" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="22" t="s">
         <v>330</v>
       </c>
       <c r="E12" s="2" t="s">
@@ -3933,11 +3934,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:9" ht="30">
       <c r="C13" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="22" t="s">
         <v>63</v>
       </c>
       <c r="E13" s="2" t="s">
@@ -3947,11 +3948,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:9" ht="30">
       <c r="C14" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="22" t="s">
         <v>340</v>
       </c>
       <c r="E14" s="2" t="s">
@@ -3961,11 +3962,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="3:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:9" ht="60">
       <c r="C15" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="22" t="s">
         <v>370</v>
       </c>
       <c r="E15" s="2" t="s">
@@ -3975,11 +3976,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="3:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:9" ht="45">
       <c r="C16" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="22" t="s">
         <v>46</v>
       </c>
       <c r="E16" s="2" t="s">
@@ -3989,11 +3990,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:6" ht="30">
       <c r="C17" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="22" t="s">
         <v>51</v>
       </c>
       <c r="E17" s="2" t="s">
@@ -4003,11 +4004,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:6" ht="30">
       <c r="C18" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="22" t="s">
         <v>52</v>
       </c>
       <c r="E18" s="2" t="s">
@@ -4017,11 +4018,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:6" ht="30">
       <c r="C19" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="22" t="s">
         <v>53</v>
       </c>
       <c r="E19" s="2" t="s">
@@ -4031,11 +4032,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:6" ht="30">
       <c r="C20" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="22" t="s">
         <v>54</v>
       </c>
       <c r="E20" s="2" t="s">
@@ -4045,11 +4046,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:6" ht="30">
       <c r="C21" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="22" t="s">
         <v>64</v>
       </c>
       <c r="E21" s="2" t="s">
@@ -4059,11 +4060,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:6" ht="45">
       <c r="C22" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="22" t="s">
         <v>55</v>
       </c>
       <c r="E22" s="2" t="s">
@@ -4073,11 +4074,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:6" ht="30">
       <c r="C23" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="22" t="s">
         <v>61</v>
       </c>
       <c r="E23" s="2" t="s">
@@ -4087,11 +4088,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:6" ht="30">
       <c r="C24" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="22" t="s">
         <v>62</v>
       </c>
       <c r="E24" s="2" t="s">
@@ -4101,11 +4102,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:6" ht="45">
       <c r="C25" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D25" s="28" t="s">
+      <c r="D25" s="22" t="s">
         <v>349</v>
       </c>
       <c r="E25" s="2" t="s">
@@ -4115,11 +4116,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:6" ht="30">
       <c r="C26" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D26" s="28" t="s">
+      <c r="D26" s="22" t="s">
         <v>351</v>
       </c>
       <c r="E26" s="2" t="s">
@@ -4129,11 +4130,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:6" ht="30">
       <c r="C27" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="22" t="s">
         <v>182</v>
       </c>
       <c r="E27" s="2" t="s">
@@ -4143,11 +4144,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:6" ht="30">
       <c r="C28" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="22" t="s">
         <v>71</v>
       </c>
       <c r="E28" s="2" t="s">
@@ -4157,11 +4158,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:6" ht="30">
       <c r="C29" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D29" s="28" t="s">
+      <c r="D29" s="22" t="s">
         <v>352</v>
       </c>
       <c r="E29" s="2" t="s">
@@ -4171,11 +4172,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:6" ht="45">
       <c r="C30" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="22" t="s">
         <v>72</v>
       </c>
       <c r="E30" s="2" t="s">
@@ -4185,11 +4186,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:6" ht="30">
       <c r="C31" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="22" t="s">
         <v>185</v>
       </c>
       <c r="E31" s="2" t="s">
@@ -4199,11 +4200,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:6" ht="45">
       <c r="C32" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="22" t="s">
         <v>113</v>
       </c>
       <c r="E32" s="2" t="s">
@@ -4213,11 +4214,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:6" ht="30">
       <c r="C33" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="22" t="s">
         <v>66</v>
       </c>
       <c r="E33" s="2" t="s">
@@ -4227,11 +4228,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:6" ht="30">
       <c r="C34" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="22" t="s">
         <v>69</v>
       </c>
       <c r="E34" s="2" t="s">
@@ -4241,11 +4242,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:6" ht="30">
       <c r="C35" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="22" t="s">
         <v>184</v>
       </c>
       <c r="E35" s="2" t="s">
@@ -4255,11 +4256,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:6" ht="30">
       <c r="C36" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="22" t="s">
         <v>369</v>
       </c>
       <c r="E36" s="2" t="s">
@@ -4269,11 +4270,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:6" ht="45">
       <c r="C37" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="22" t="s">
         <v>47</v>
       </c>
       <c r="E37" s="2" t="s">
@@ -4283,11 +4284,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:6" ht="45">
       <c r="C38" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="22" t="s">
         <v>65</v>
       </c>
       <c r="E38" s="2" t="s">
@@ -4297,11 +4298,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:6" ht="45">
       <c r="C39" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="22" t="s">
         <v>68</v>
       </c>
       <c r="E39" s="2" t="s">
@@ -4311,11 +4312,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:6" ht="45">
       <c r="C40" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="D40" s="22" t="s">
         <v>350</v>
       </c>
       <c r="E40" s="2" t="s">
@@ -4325,11 +4326,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:6" ht="30">
       <c r="C41" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" s="22" t="s">
         <v>207</v>
       </c>
       <c r="E41" s="2" t="s">
@@ -4339,11 +4340,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:6" ht="30">
       <c r="C42" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D42" s="22" t="s">
         <v>58</v>
       </c>
       <c r="E42" s="2" t="s">
@@ -4353,11 +4354,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:6" ht="45">
       <c r="C43" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D43" s="28" t="s">
+      <c r="D43" s="22" t="s">
         <v>353</v>
       </c>
       <c r="E43" s="2" t="s">
@@ -4367,11 +4368,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:6" ht="30">
       <c r="C44" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D44" s="22" t="s">
         <v>44</v>
       </c>
       <c r="E44" s="2" t="s">
@@ -4381,11 +4382,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:6" ht="30">
       <c r="C45" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D45" s="22" t="s">
         <v>217</v>
       </c>
       <c r="E45" s="2" t="s">
@@ -4395,11 +4396,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:6" ht="30">
       <c r="C46" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D46" s="22" t="s">
         <v>59</v>
       </c>
       <c r="E46" s="2" t="s">
@@ -4409,11 +4410,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:6" ht="30">
       <c r="C47" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="D47" s="22" t="s">
         <v>221</v>
       </c>
       <c r="E47" s="2" t="s">
@@ -4423,11 +4424,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:6" ht="30">
       <c r="C48" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="D48" s="22" t="s">
         <v>60</v>
       </c>
       <c r="E48" s="2" t="s">
@@ -4437,11 +4438,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:6" ht="30">
       <c r="C49" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D49" s="22" t="s">
         <v>407</v>
       </c>
       <c r="E49" s="2" t="s">
@@ -4451,11 +4452,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:6" ht="30">
       <c r="C50" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="D50" s="22" t="s">
         <v>408</v>
       </c>
       <c r="E50" s="2" t="s">
@@ -4465,11 +4466,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="3:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:6" ht="75">
       <c r="C51" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D51" s="5" t="s">
+      <c r="D51" s="22" t="s">
         <v>360</v>
       </c>
       <c r="E51" s="2" t="s">
@@ -4479,11 +4480,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="3:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:6" ht="60">
       <c r="C52" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="D52" s="5" t="s">
+      <c r="D52" s="22" t="s">
         <v>359</v>
       </c>
       <c r="E52" s="2" t="s">
@@ -4493,11 +4494,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="3:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:6" ht="60">
       <c r="C53" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="D53" s="28" t="s">
+      <c r="D53" s="22" t="s">
         <v>356</v>
       </c>
       <c r="E53" s="2" t="s">
@@ -4507,11 +4508,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:6" ht="45">
       <c r="C54" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="D54" s="28" t="s">
+      <c r="D54" s="22" t="s">
         <v>362</v>
       </c>
       <c r="E54" s="2" t="s">
@@ -4521,11 +4522,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:6" ht="30">
       <c r="C55" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="D55" s="28" t="s">
+      <c r="D55" s="22" t="s">
         <v>361</v>
       </c>
       <c r="E55" s="2" t="s">
@@ -4535,11 +4536,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:6" ht="45">
       <c r="C56" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="D56" s="28" t="s">
+      <c r="D56" s="22" t="s">
         <v>357</v>
       </c>
       <c r="E56" s="2" t="s">
@@ -4549,7 +4550,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:6" ht="45">
       <c r="C57" s="7" t="s">
         <v>345</v>
       </c>
@@ -4563,11 +4564,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:6">
       <c r="C58" s="7" t="s">
         <v>371</v>
       </c>
-      <c r="D58" s="5" t="s">
+      <c r="D58" s="22" t="s">
         <v>251</v>
       </c>
       <c r="E58" s="2" t="s">
@@ -4586,22 +4587,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D3:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="3" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:5">
       <c r="D3" s="35" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="36"/>
     </row>
-    <row r="4" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:5">
       <c r="D4" s="1">
         <v>1</v>
       </c>
@@ -4609,7 +4610,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:5">
       <c r="D5" s="1">
         <v>2</v>
       </c>
@@ -4617,7 +4618,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:5">
       <c r="D6" s="1">
         <v>3</v>
       </c>
@@ -4625,13 +4626,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:5">
       <c r="D9" s="35" t="s">
         <v>4</v>
       </c>
       <c r="E9" s="36"/>
     </row>
-    <row r="10" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:5">
       <c r="D10" s="1">
         <v>1</v>
       </c>
@@ -4639,7 +4640,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:5">
       <c r="D11" s="1">
         <v>2</v>
       </c>
@@ -4647,7 +4648,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:5">
       <c r="D12" s="1">
         <v>3</v>
       </c>
@@ -4655,13 +4656,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:5">
       <c r="D15" s="34" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="34"/>
     </row>
-    <row r="16" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="4:5">
       <c r="D16" s="1" t="s">
         <v>12</v>
       </c>
@@ -4669,7 +4670,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:5">
       <c r="D17" s="1" t="s">
         <v>13</v>
       </c>
@@ -4688,14 +4689,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.85546875" customWidth="1"/>
     <col min="2" max="2" width="4.42578125" customWidth="1"/>
@@ -4703,7 +4704,7 @@
     <col min="4" max="4" width="78.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:5">
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4714,7 +4715,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:5">
       <c r="C2" s="7" t="s">
         <v>372</v>
       </c>
@@ -4725,7 +4726,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:5">
       <c r="C3" s="7" t="s">
         <v>390</v>
       </c>
@@ -4736,7 +4737,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:5">
       <c r="C4" s="7" t="s">
         <v>391</v>
       </c>
@@ -4747,7 +4748,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:5">
       <c r="C5" s="7" t="s">
         <v>392</v>
       </c>
@@ -4758,7 +4759,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:5" ht="30">
       <c r="C6" s="7" t="s">
         <v>393</v>
       </c>
@@ -4769,7 +4770,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:5" ht="30">
       <c r="C7" s="7" t="s">
         <v>394</v>
       </c>
@@ -4780,7 +4781,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:5" ht="30">
       <c r="C8" s="7" t="s">
         <v>395</v>
       </c>
@@ -4791,7 +4792,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:5">
       <c r="C9" s="7" t="s">
         <v>396</v>
       </c>
@@ -4802,7 +4803,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="3:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:5" ht="60">
       <c r="C10" s="7" t="s">
         <v>397</v>
       </c>
@@ -4813,7 +4814,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:5">
       <c r="C11" s="7" t="s">
         <v>398</v>
       </c>
@@ -4824,7 +4825,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:5" ht="30">
       <c r="C12" s="7" t="s">
         <v>399</v>
       </c>
@@ -4835,7 +4836,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:5" ht="30">
       <c r="C13" s="7" t="s">
         <v>400</v>
       </c>
@@ -4846,7 +4847,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:5">
       <c r="C14" s="7" t="s">
         <v>401</v>
       </c>
@@ -4857,7 +4858,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:5">
       <c r="C15" s="7" t="s">
         <v>402</v>
       </c>
@@ -4868,7 +4869,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:5" ht="30">
       <c r="C16" s="7" t="s">
         <v>403</v>
       </c>
@@ -4879,7 +4880,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:5">
       <c r="C17" s="7" t="s">
         <v>404</v>
       </c>
@@ -4890,7 +4891,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:5" ht="30">
       <c r="C18" s="7" t="s">
         <v>405</v>
       </c>
@@ -4901,7 +4902,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="3:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:5" ht="45">
       <c r="C19" s="7" t="s">
         <v>409</v>
       </c>
@@ -4912,7 +4913,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:5" ht="30">
       <c r="C20" s="7" t="s">
         <v>415</v>
       </c>

</xml_diff>

<commit_message>
- HistorialTrabajos 100%: editar detalles - datepicker de jquery UI para registro de usuarios
</commit_message>
<xml_diff>
--- a/Documentación/Análisis/Lista de Requerimientos - Historias de Usuarios.xlsx
+++ b/Documentación/Análisis/Lista de Requerimientos - Historias de Usuarios.xlsx
@@ -1679,6 +1679,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1696,12 +1702,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2043,13 +2043,13 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="15"/>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="33"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="35"/>
       <c r="G3" s="16"/>
       <c r="H3" s="12"/>
     </row>
@@ -2203,16 +2203,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:J58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.42578125" customWidth="1"/>
-    <col min="2" max="2" width="2.7109375" style="37" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" style="31" customWidth="1"/>
     <col min="3" max="3" width="5.7109375" style="26" customWidth="1"/>
     <col min="4" max="4" width="37" style="21" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" style="30" bestFit="1" customWidth="1"/>
@@ -2224,7 +2225,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="31" t="s">
         <v>410</v>
       </c>
       <c r="C1" s="4" t="s">
@@ -2252,8 +2253,8 @@
         <v>315</v>
       </c>
     </row>
-    <row r="2" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B2" s="37">
+    <row r="2" spans="2:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="31">
         <v>1</v>
       </c>
       <c r="C2" s="25" t="s">
@@ -2281,8 +2282,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="B3" s="37">
+    <row r="3" spans="2:10" ht="90" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="31">
         <v>2</v>
       </c>
       <c r="C3" s="25" t="s">
@@ -2310,8 +2311,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="B4" s="37">
+    <row r="4" spans="2:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="31">
         <v>3</v>
       </c>
       <c r="C4" s="25" t="s">
@@ -2339,8 +2340,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B5" s="37">
+    <row r="5" spans="2:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="31">
         <v>4</v>
       </c>
       <c r="C5" s="25" t="s">
@@ -2368,8 +2369,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B6" s="37">
+    <row r="6" spans="2:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="31">
         <v>5</v>
       </c>
       <c r="C6" s="25" t="s">
@@ -2397,8 +2398,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="B7" s="37">
+    <row r="7" spans="2:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="31">
         <v>6</v>
       </c>
       <c r="C7" s="25" t="s">
@@ -2426,8 +2427,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="B8" s="37">
+    <row r="8" spans="2:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="31">
         <v>7</v>
       </c>
       <c r="C8" s="25" t="s">
@@ -2455,8 +2456,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="B9" s="37">
+    <row r="9" spans="2:10" ht="75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="31">
         <v>8</v>
       </c>
       <c r="C9" s="25" t="s">
@@ -2484,8 +2485,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="B10" s="37">
+    <row r="10" spans="2:10" ht="75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="31">
         <v>9</v>
       </c>
       <c r="C10" s="25" t="s">
@@ -2513,8 +2514,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B11" s="37">
+    <row r="11" spans="2:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="31">
         <v>10</v>
       </c>
       <c r="C11" s="25" t="s">
@@ -2542,256 +2543,256 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="B12" s="37">
-        <v>11</v>
+    <row r="12" spans="2:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="B12" s="32">
+        <v>15</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>168</v>
+        <v>143</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>166</v>
+        <v>141</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>167</v>
+        <v>142</v>
       </c>
       <c r="H12" s="25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I12" s="25">
         <v>3</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="B13" s="37">
-        <v>12</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B13" s="32">
+        <v>18</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="E13" s="29" t="s">
         <v>10</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>132</v>
+        <v>150</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="H13" s="25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I13" s="25">
         <v>2</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B14" s="38">
-        <v>13</v>
+      <c r="B14" s="32">
+        <v>19</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>338</v>
+        <v>153</v>
       </c>
       <c r="E14" s="29" t="s">
         <v>10</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>336</v>
+        <v>136</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>337</v>
+        <v>137</v>
       </c>
       <c r="H14" s="25">
+        <v>3</v>
+      </c>
+      <c r="I14" s="25">
         <v>1</v>
       </c>
-      <c r="I14" s="25">
-        <v>2</v>
-      </c>
       <c r="J14" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B15" s="38">
-        <v>14</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="32">
+        <v>25</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>273</v>
+        <v>284</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>135</v>
+        <v>171</v>
       </c>
       <c r="E15" s="29" t="s">
-        <v>10</v>
+        <v>118</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>133</v>
+        <v>169</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>134</v>
+        <v>170</v>
       </c>
       <c r="H15" s="25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I15" s="25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="B16" s="38">
-        <v>15</v>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" ht="75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="32">
+        <v>33</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>274</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>143</v>
+        <v>292</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>253</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>10</v>
+        <v>323</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>141</v>
+        <v>251</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>142</v>
+        <v>252</v>
       </c>
       <c r="H16" s="25">
         <v>3</v>
       </c>
       <c r="I16" s="25">
+        <v>2</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="32">
+        <v>34</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>293</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>323</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="H17" s="25">
         <v>3</v>
       </c>
-      <c r="J16" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="B17" s="38">
-        <v>16</v>
-      </c>
-      <c r="C17" s="25" t="s">
-        <v>275</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="E17" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="H17" s="25">
+      <c r="I17" s="25">
         <v>1</v>
       </c>
-      <c r="I17" s="25">
+      <c r="J17" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="32">
+        <v>35</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>294</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="E18" s="29" t="s">
+        <v>323</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="H18" s="25">
         <v>3</v>
       </c>
-      <c r="J17" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B18" s="38">
-        <v>17</v>
-      </c>
-      <c r="C18" s="25" t="s">
-        <v>276</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>320</v>
-      </c>
-      <c r="E18" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="H18" s="25">
+      <c r="I18" s="25">
         <v>1</v>
       </c>
-      <c r="I18" s="25">
-        <v>3</v>
-      </c>
       <c r="J18" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B19" s="38">
-        <v>18</v>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="32">
+        <v>36</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>277</v>
+        <v>295</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>151</v>
+        <v>195</v>
       </c>
       <c r="E19" s="29" t="s">
-        <v>10</v>
+        <v>323</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>150</v>
+        <v>193</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>152</v>
+        <v>194</v>
       </c>
       <c r="H19" s="25">
         <v>3</v>
       </c>
       <c r="I19" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B20" s="38">
-        <v>19</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="32">
+        <v>41</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>278</v>
+        <v>300</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>153</v>
+        <v>260</v>
       </c>
       <c r="E20" s="29" t="s">
-        <v>10</v>
+        <v>323</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>136</v>
+        <v>207</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>137</v>
+        <v>208</v>
       </c>
       <c r="H20" s="25">
         <v>3</v>
@@ -2800,230 +2801,230 @@
         <v>1</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B21" s="38">
-        <v>20</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="32">
+        <v>43</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>279</v>
+        <v>302</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>156</v>
+        <v>211</v>
       </c>
       <c r="E21" s="29" t="s">
-        <v>10</v>
+        <v>323</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>154</v>
+        <v>210</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>155</v>
+        <v>212</v>
       </c>
       <c r="H21" s="25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I21" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="B22" s="38">
-        <v>21</v>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="32">
+        <v>45</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>280</v>
+        <v>304</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>158</v>
+        <v>258</v>
       </c>
       <c r="E22" s="29" t="s">
-        <v>10</v>
+        <v>323</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>157</v>
+        <v>217</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>326</v>
+        <v>212</v>
       </c>
       <c r="H22" s="25">
+        <v>3</v>
+      </c>
+      <c r="I22" s="25">
         <v>2</v>
       </c>
-      <c r="I22" s="25">
+      <c r="J22" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" ht="75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="32">
+        <v>46</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>305</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>323</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="H23" s="25">
         <v>3</v>
       </c>
-      <c r="J22" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="B23" s="38">
-        <v>22</v>
-      </c>
-      <c r="C23" s="25" t="s">
-        <v>281</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="E23" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="H23" s="25">
-        <v>1</v>
-      </c>
       <c r="I23" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="B24" s="38">
-        <v>23</v>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="32">
+        <v>47</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>282</v>
+        <v>306</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>318</v>
+        <v>222</v>
       </c>
       <c r="E24" s="29" t="s">
-        <v>10</v>
+        <v>323</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>162</v>
+        <v>221</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>163</v>
+        <v>225</v>
       </c>
       <c r="H24" s="25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I24" s="25">
         <v>1</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="B25" s="38">
-        <v>24</v>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="32">
+        <v>49</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>283</v>
+        <v>308</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>349</v>
+        <v>404</v>
       </c>
       <c r="E25" s="29" t="s">
+        <v>323</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="H25" s="25">
+        <v>3</v>
+      </c>
+      <c r="I25" s="25">
+        <v>3</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B26" s="32">
+        <v>14</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>273</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E26" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="F25" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="H25" s="25">
-        <v>1</v>
-      </c>
-      <c r="I25" s="25">
+      <c r="F26" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="H26" s="25">
         <v>2</v>
       </c>
-      <c r="J25" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B26" s="38">
-        <v>25</v>
-      </c>
-      <c r="C26" s="25" t="s">
-        <v>284</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="E26" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="H26" s="25">
-        <v>3</v>
-      </c>
       <c r="I26" s="25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>77</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="2:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="B27" s="38">
-        <v>26</v>
+      <c r="B27" s="32">
+        <v>21</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>324</v>
+        <v>158</v>
       </c>
       <c r="E27" s="29" t="s">
-        <v>118</v>
+        <v>10</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>180</v>
+        <v>157</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>256</v>
+        <v>326</v>
       </c>
       <c r="H27" s="25">
         <v>2</v>
       </c>
       <c r="I27" s="25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="B28" s="38">
-        <v>27</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="32">
+        <v>26</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>174</v>
+        <v>324</v>
       </c>
       <c r="E28" s="29" t="s">
         <v>118</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>173</v>
+        <v>256</v>
       </c>
       <c r="H28" s="25">
         <v>2</v>
@@ -3032,27 +3033,27 @@
         <v>2</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B29" s="38">
-        <v>28</v>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" ht="75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="32">
+        <v>27</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>257</v>
+        <v>174</v>
       </c>
       <c r="E29" s="29" t="s">
         <v>118</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>254</v>
+        <v>173</v>
       </c>
       <c r="H29" s="25">
         <v>2</v>
@@ -3061,40 +3062,40 @@
         <v>2</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="B30" s="38">
-        <v>29</v>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="32">
+        <v>28</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>178</v>
+        <v>257</v>
       </c>
       <c r="E30" s="29" t="s">
         <v>118</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>177</v>
+        <v>254</v>
       </c>
       <c r="H30" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I30" s="25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B31" s="38">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="32">
         <v>30</v>
       </c>
       <c r="C31" s="25" t="s">
@@ -3122,198 +3123,198 @@
         <v>82</v>
       </c>
     </row>
-    <row r="32" spans="2:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="B32" s="38">
-        <v>31</v>
+    <row r="32" spans="2:10" ht="75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="32">
+        <v>37</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="E32" s="29" t="s">
-        <v>118</v>
+        <v>323</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="H32" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I32" s="25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J32" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="B33" s="38">
-        <v>32</v>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="32">
+        <v>42</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>291</v>
+        <v>301</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
       <c r="E33" s="29" t="s">
-        <v>118</v>
+        <v>323</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>244</v>
+        <v>209</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>246</v>
+        <v>197</v>
       </c>
       <c r="H33" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I33" s="25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J33" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="B34" s="38">
-        <v>33</v>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="32">
+        <v>50</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>292</v>
-      </c>
-      <c r="D34" s="22" t="s">
-        <v>253</v>
+        <v>309</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>229</v>
       </c>
       <c r="E34" s="29" t="s">
         <v>323</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>251</v>
+        <v>228</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>252</v>
+        <v>358</v>
       </c>
       <c r="H34" s="25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I34" s="25">
         <v>2</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B35" s="38">
-        <v>34</v>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B35" s="32">
+        <v>51</v>
       </c>
       <c r="C35" s="25" t="s">
-        <v>293</v>
+        <v>310</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>189</v>
+        <v>237</v>
       </c>
       <c r="E35" s="29" t="s">
-        <v>323</v>
+        <v>10</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>187</v>
+        <v>230</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>188</v>
+        <v>231</v>
       </c>
       <c r="H35" s="25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I35" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="36" spans="2:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="B36" s="38">
-        <v>35</v>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="32">
+        <v>53</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>294</v>
+        <v>312</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>191</v>
+        <v>235</v>
       </c>
       <c r="E36" s="29" t="s">
-        <v>323</v>
+        <v>118</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>192</v>
+        <v>233</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>190</v>
+        <v>234</v>
       </c>
       <c r="H36" s="25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I36" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J36" s="7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="37" spans="2:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="B37" s="38">
-        <v>36</v>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="32">
+        <v>54</v>
       </c>
       <c r="C37" s="25" t="s">
-        <v>295</v>
+        <v>313</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>195</v>
+        <v>239</v>
       </c>
       <c r="E37" s="29" t="s">
-        <v>323</v>
+        <v>118</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>193</v>
+        <v>240</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>194</v>
+        <v>238</v>
       </c>
       <c r="H37" s="25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I37" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J37" s="7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="38" spans="2:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="B38" s="38">
-        <v>37</v>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="32">
+        <v>55</v>
       </c>
       <c r="C38" s="25" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>198</v>
+        <v>243</v>
       </c>
       <c r="E38" s="29" t="s">
         <v>323</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>196</v>
+        <v>241</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>197</v>
+        <v>242</v>
       </c>
       <c r="H38" s="25">
         <v>2</v>
@@ -3322,201 +3323,201 @@
         <v>2</v>
       </c>
       <c r="J38" s="7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="39" spans="2:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="B39" s="38">
-        <v>38</v>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="32">
+        <v>56</v>
       </c>
       <c r="C39" s="25" t="s">
-        <v>297</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>201</v>
+        <v>339</v>
+      </c>
+      <c r="D39" s="22" t="s">
+        <v>362</v>
       </c>
       <c r="E39" s="29" t="s">
         <v>323</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>199</v>
+        <v>360</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>200</v>
+        <v>361</v>
       </c>
       <c r="H39" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I39" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J39" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="40" spans="2:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="B40" s="38">
-        <v>39</v>
+        <v>340</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" ht="75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="31">
+        <v>11</v>
       </c>
       <c r="C40" s="25" t="s">
-        <v>298</v>
+        <v>270</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>321</v>
+        <v>168</v>
       </c>
       <c r="E40" s="29" t="s">
-        <v>323</v>
+        <v>117</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>202</v>
+        <v>166</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>203</v>
+        <v>167</v>
       </c>
       <c r="H40" s="25">
         <v>1</v>
       </c>
       <c r="I40" s="25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J40" s="7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="41" spans="2:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="B41" s="38">
-        <v>40</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="B41" s="31">
+        <v>12</v>
       </c>
       <c r="C41" s="25" t="s">
-        <v>299</v>
+        <v>271</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>319</v>
+        <v>161</v>
       </c>
       <c r="E41" s="29" t="s">
-        <v>323</v>
+        <v>10</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>205</v>
+        <v>132</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>206</v>
+        <v>140</v>
       </c>
       <c r="H41" s="25">
         <v>1</v>
       </c>
       <c r="I41" s="25">
+        <v>2</v>
+      </c>
+      <c r="J41" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B42" s="32">
+        <v>13</v>
+      </c>
+      <c r="C42" s="25" t="s">
+        <v>272</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="E42" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="H42" s="25">
+        <v>1</v>
+      </c>
+      <c r="I42" s="25">
+        <v>2</v>
+      </c>
+      <c r="J42" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="B43" s="32">
+        <v>16</v>
+      </c>
+      <c r="C43" s="25" t="s">
+        <v>275</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="E43" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="H43" s="25">
+        <v>1</v>
+      </c>
+      <c r="I43" s="25">
         <v>3</v>
       </c>
-      <c r="J41" s="7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="42" spans="2:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="B42" s="38">
-        <v>41</v>
-      </c>
-      <c r="C42" s="25" t="s">
-        <v>300</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="E42" s="29" t="s">
-        <v>323</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="H42" s="25">
+      <c r="J43" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B44" s="32">
+        <v>17</v>
+      </c>
+      <c r="C44" s="25" t="s">
+        <v>276</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="E44" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="H44" s="25">
+        <v>1</v>
+      </c>
+      <c r="I44" s="25">
         <v>3</v>
       </c>
-      <c r="I42" s="25">
-        <v>1</v>
-      </c>
-      <c r="J42" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="43" spans="2:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="B43" s="38">
-        <v>42</v>
-      </c>
-      <c r="C43" s="25" t="s">
-        <v>301</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="E43" s="29" t="s">
-        <v>323</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="H43" s="25">
-        <v>2</v>
-      </c>
-      <c r="I43" s="25">
-        <v>2</v>
-      </c>
-      <c r="J43" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="44" spans="2:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="B44" s="38">
-        <v>43</v>
-      </c>
-      <c r="C44" s="25" t="s">
-        <v>302</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="E44" s="29" t="s">
-        <v>323</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="H44" s="25">
-        <v>3</v>
-      </c>
-      <c r="I44" s="25">
-        <v>2</v>
-      </c>
       <c r="J44" s="7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="45" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B45" s="38">
-        <v>44</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B45" s="32">
+        <v>20</v>
       </c>
       <c r="C45" s="25" t="s">
-        <v>303</v>
+        <v>279</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>216</v>
+        <v>156</v>
       </c>
       <c r="E45" s="29" t="s">
-        <v>323</v>
+        <v>10</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>213</v>
+        <v>154</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>215</v>
+        <v>155</v>
       </c>
       <c r="H45" s="25">
         <v>1</v>
@@ -3525,359 +3526,359 @@
         <v>1</v>
       </c>
       <c r="J45" s="7" t="s">
-        <v>96</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="2:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="B46" s="38">
-        <v>45</v>
+      <c r="B46" s="32">
+        <v>22</v>
       </c>
       <c r="C46" s="25" t="s">
-        <v>304</v>
+        <v>281</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>258</v>
+        <v>317</v>
       </c>
       <c r="E46" s="29" t="s">
-        <v>323</v>
+        <v>10</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>217</v>
+        <v>159</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>212</v>
+        <v>160</v>
       </c>
       <c r="H46" s="25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I46" s="25">
+        <v>1</v>
+      </c>
+      <c r="J46" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="B47" s="32">
+        <v>23</v>
+      </c>
+      <c r="C47" s="25" t="s">
+        <v>282</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="E47" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="H47" s="25">
+        <v>1</v>
+      </c>
+      <c r="I47" s="25">
+        <v>1</v>
+      </c>
+      <c r="J47" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="B48" s="32">
+        <v>24</v>
+      </c>
+      <c r="C48" s="25" t="s">
+        <v>283</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="E48" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="H48" s="25">
+        <v>1</v>
+      </c>
+      <c r="I48" s="25">
         <v>2</v>
       </c>
-      <c r="J46" s="7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="47" spans="2:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="B47" s="38">
-        <v>46</v>
-      </c>
-      <c r="C47" s="25" t="s">
-        <v>305</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="E47" s="29" t="s">
-        <v>323</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="H47" s="25">
-        <v>3</v>
-      </c>
-      <c r="I47" s="25">
-        <v>2</v>
-      </c>
-      <c r="J47" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="48" spans="2:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="B48" s="38">
-        <v>47</v>
-      </c>
-      <c r="C48" s="25" t="s">
-        <v>306</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="E48" s="29" t="s">
-        <v>323</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="G48" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="H48" s="25">
-        <v>3</v>
-      </c>
-      <c r="I48" s="25">
-        <v>1</v>
-      </c>
       <c r="J48" s="7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="49" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B49" s="38">
-        <v>48</v>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10" ht="75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="32">
+        <v>29</v>
       </c>
       <c r="C49" s="25" t="s">
-        <v>307</v>
+        <v>288</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>227</v>
+        <v>178</v>
       </c>
       <c r="E49" s="29" t="s">
-        <v>323</v>
+        <v>118</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>223</v>
+        <v>176</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>226</v>
+        <v>177</v>
       </c>
       <c r="H49" s="25">
         <v>1</v>
       </c>
       <c r="I49" s="25">
+        <v>3</v>
+      </c>
+      <c r="J49" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" ht="90" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="32">
+        <v>31</v>
+      </c>
+      <c r="C50" s="25" t="s">
+        <v>290</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="E50" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="H50" s="25">
         <v>1</v>
-      </c>
-      <c r="J49" s="7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="50" spans="2:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="B50" s="38">
-        <v>49</v>
-      </c>
-      <c r="C50" s="25" t="s">
-        <v>308</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>404</v>
-      </c>
-      <c r="E50" s="29" t="s">
-        <v>323</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>405</v>
-      </c>
-      <c r="G50" s="5" t="s">
-        <v>406</v>
-      </c>
-      <c r="H50" s="25">
-        <v>3</v>
       </c>
       <c r="I50" s="25">
         <v>3</v>
       </c>
       <c r="J50" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="51" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B51" s="38">
-        <v>50</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="32">
+        <v>32</v>
       </c>
       <c r="C51" s="25" t="s">
-        <v>309</v>
+        <v>291</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>229</v>
+        <v>245</v>
       </c>
       <c r="E51" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="H51" s="25">
+        <v>1</v>
+      </c>
+      <c r="I51" s="25">
+        <v>3</v>
+      </c>
+      <c r="J51" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" ht="75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="32">
+        <v>38</v>
+      </c>
+      <c r="C52" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="E52" s="29" t="s">
         <v>323</v>
       </c>
-      <c r="F51" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="G51" s="5" t="s">
-        <v>358</v>
-      </c>
-      <c r="H51" s="25">
-        <v>2</v>
-      </c>
-      <c r="I51" s="25">
-        <v>2</v>
-      </c>
-      <c r="J51" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="52" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B52" s="38">
-        <v>51</v>
-      </c>
-      <c r="C52" s="25" t="s">
-        <v>310</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="E52" s="29" t="s">
-        <v>10</v>
-      </c>
       <c r="F52" s="5" t="s">
-        <v>230</v>
+        <v>199</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>231</v>
+        <v>200</v>
       </c>
       <c r="H52" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I52" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J52" s="7" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="53" spans="2:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="B53" s="38">
-        <v>52</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10" ht="75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="32">
+        <v>39</v>
       </c>
       <c r="C53" s="25" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>236</v>
+        <v>321</v>
       </c>
       <c r="E53" s="29" t="s">
-        <v>10</v>
+        <v>323</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>232</v>
+        <v>202</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>359</v>
+        <v>203</v>
       </c>
       <c r="H53" s="25">
         <v>1</v>
       </c>
       <c r="I53" s="25">
+        <v>2</v>
+      </c>
+      <c r="J53" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="32">
+        <v>40</v>
+      </c>
+      <c r="C54" s="25" t="s">
+        <v>299</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="E54" s="29" t="s">
+        <v>323</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="H54" s="25">
+        <v>1</v>
+      </c>
+      <c r="I54" s="25">
         <v>3</v>
       </c>
-      <c r="J53" s="7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="54" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B54" s="38">
-        <v>53</v>
-      </c>
-      <c r="C54" s="25" t="s">
-        <v>312</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="E54" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="G54" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="H54" s="25">
-        <v>2</v>
-      </c>
-      <c r="I54" s="25">
-        <v>2</v>
-      </c>
       <c r="J54" s="7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="55" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B55" s="38">
-        <v>54</v>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="55" spans="2:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="32">
+        <v>44</v>
       </c>
       <c r="C55" s="25" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>239</v>
+        <v>216</v>
       </c>
       <c r="E55" s="29" t="s">
-        <v>118</v>
+        <v>323</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>240</v>
+        <v>213</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>238</v>
+        <v>215</v>
       </c>
       <c r="H55" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I55" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J55" s="7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="56" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B56" s="38">
-        <v>55</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="32">
+        <v>48</v>
       </c>
       <c r="C56" s="25" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="E56" s="29" t="s">
         <v>323</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>241</v>
+        <v>223</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
       <c r="H56" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I56" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J56" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="57" spans="2:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="B57" s="38">
-        <v>56</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="2:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="B57" s="32">
+        <v>52</v>
       </c>
       <c r="C57" s="25" t="s">
-        <v>339</v>
-      </c>
-      <c r="D57" s="22" t="s">
-        <v>362</v>
+        <v>311</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>236</v>
       </c>
       <c r="E57" s="29" t="s">
-        <v>323</v>
+        <v>10</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>360</v>
+        <v>232</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="H57" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I57" s="25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J57" s="7" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="58" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B58" s="38">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="32">
         <v>57</v>
       </c>
       <c r="C58" s="25" t="s">
@@ -3907,12 +3908,17 @@
     </row>
   </sheetData>
   <autoFilter ref="C1:J58">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Proveedor"/>
+      </filters>
+    </filterColumn>
     <sortState ref="C2:J58">
       <sortCondition ref="C1:C58"/>
     </sortState>
   </autoFilter>
   <sortState ref="B2:J58">
-    <sortCondition ref="B2:B58"/>
+    <sortCondition descending="1" ref="H2:H58"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3923,14 +3929,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.42578125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="2.7109375" style="37" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" style="31" customWidth="1"/>
     <col min="3" max="3" width="5.42578125" style="8" customWidth="1"/>
     <col min="4" max="4" width="78.7109375" style="6" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" style="8" customWidth="1"/>
@@ -3941,7 +3947,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="31" t="s">
         <v>410</v>
       </c>
       <c r="C1" s="3" t="s">
@@ -3958,7 +3964,7 @@
       </c>
     </row>
     <row r="2" spans="2:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B2" s="37">
+      <c r="B2" s="31">
         <v>1</v>
       </c>
       <c r="C2" s="7" t="s">
@@ -3982,7 +3988,7 @@
       </c>
     </row>
     <row r="3" spans="2:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B3" s="37">
+      <c r="B3" s="31">
         <v>2</v>
       </c>
       <c r="C3" s="7" t="s">
@@ -4006,7 +4012,7 @@
       </c>
     </row>
     <row r="4" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="37">
+      <c r="B4" s="31">
         <v>3</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -4030,7 +4036,7 @@
       </c>
     </row>
     <row r="5" spans="2:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B5" s="37">
+      <c r="B5" s="31">
         <v>4</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -4047,7 +4053,7 @@
       </c>
     </row>
     <row r="6" spans="2:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B6" s="37">
+      <c r="B6" s="31">
         <v>5</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -4064,7 +4070,7 @@
       </c>
     </row>
     <row r="7" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="37">
+      <c r="B7" s="31">
         <v>6</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -4081,7 +4087,7 @@
       </c>
     </row>
     <row r="8" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="37">
+      <c r="B8" s="31">
         <v>7</v>
       </c>
       <c r="C8" s="7" t="s">
@@ -4098,7 +4104,7 @@
       </c>
     </row>
     <row r="9" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="37">
+      <c r="B9" s="31">
         <v>8</v>
       </c>
       <c r="C9" s="7" t="s">
@@ -4115,7 +4121,7 @@
       </c>
     </row>
     <row r="10" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="37">
+      <c r="B10" s="31">
         <v>9</v>
       </c>
       <c r="C10" s="7" t="s">
@@ -4132,7 +4138,7 @@
       </c>
     </row>
     <row r="11" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="37">
+      <c r="B11" s="31">
         <v>10</v>
       </c>
       <c r="C11" s="7" t="s">
@@ -4149,7 +4155,7 @@
       </c>
     </row>
     <row r="12" spans="2:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B12" s="37">
+      <c r="B12" s="31">
         <v>11</v>
       </c>
       <c r="C12" s="7" t="s">
@@ -4166,7 +4172,7 @@
       </c>
     </row>
     <row r="13" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="37">
+      <c r="B13" s="31">
         <v>12</v>
       </c>
       <c r="C13" s="7" t="s">
@@ -4183,7 +4189,7 @@
       </c>
     </row>
     <row r="14" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="38">
+      <c r="B14" s="32">
         <v>13</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -4200,7 +4206,7 @@
       </c>
     </row>
     <row r="15" spans="2:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B15" s="38">
+      <c r="B15" s="32">
         <v>14</v>
       </c>
       <c r="C15" s="7" t="s">
@@ -4217,7 +4223,7 @@
       </c>
     </row>
     <row r="16" spans="2:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B16" s="38">
+      <c r="B16" s="32">
         <v>15</v>
       </c>
       <c r="C16" s="7" t="s">
@@ -4234,7 +4240,7 @@
       </c>
     </row>
     <row r="17" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B17" s="38">
+      <c r="B17" s="32">
         <v>16</v>
       </c>
       <c r="C17" s="7" t="s">
@@ -4251,7 +4257,7 @@
       </c>
     </row>
     <row r="18" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="38">
+      <c r="B18" s="32">
         <v>17</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -4268,7 +4274,7 @@
       </c>
     </row>
     <row r="19" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B19" s="38">
+      <c r="B19" s="32">
         <v>18</v>
       </c>
       <c r="C19" s="7" t="s">
@@ -4285,7 +4291,7 @@
       </c>
     </row>
     <row r="20" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B20" s="38">
+      <c r="B20" s="32">
         <v>19</v>
       </c>
       <c r="C20" s="7" t="s">
@@ -4302,7 +4308,7 @@
       </c>
     </row>
     <row r="21" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B21" s="38">
+      <c r="B21" s="32">
         <v>20</v>
       </c>
       <c r="C21" s="7" t="s">
@@ -4319,7 +4325,7 @@
       </c>
     </row>
     <row r="22" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B22" s="38">
+      <c r="B22" s="32">
         <v>21</v>
       </c>
       <c r="C22" s="7" t="s">
@@ -4336,7 +4342,7 @@
       </c>
     </row>
     <row r="23" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B23" s="38">
+      <c r="B23" s="32">
         <v>22</v>
       </c>
       <c r="C23" s="7" t="s">
@@ -4353,7 +4359,7 @@
       </c>
     </row>
     <row r="24" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B24" s="38">
+      <c r="B24" s="32">
         <v>23</v>
       </c>
       <c r="C24" s="7" t="s">
@@ -4370,7 +4376,7 @@
       </c>
     </row>
     <row r="25" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B25" s="38">
+      <c r="B25" s="32">
         <v>24</v>
       </c>
       <c r="C25" s="7" t="s">
@@ -4387,7 +4393,7 @@
       </c>
     </row>
     <row r="26" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B26" s="38">
+      <c r="B26" s="32">
         <v>25</v>
       </c>
       <c r="C26" s="7" t="s">
@@ -4404,7 +4410,7 @@
       </c>
     </row>
     <row r="27" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B27" s="38">
+      <c r="B27" s="32">
         <v>26</v>
       </c>
       <c r="C27" s="7" t="s">
@@ -4421,7 +4427,7 @@
       </c>
     </row>
     <row r="28" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B28" s="38">
+      <c r="B28" s="32">
         <v>27</v>
       </c>
       <c r="C28" s="7" t="s">
@@ -4438,7 +4444,7 @@
       </c>
     </row>
     <row r="29" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B29" s="38">
+      <c r="B29" s="32">
         <v>28</v>
       </c>
       <c r="C29" s="7" t="s">
@@ -4455,7 +4461,7 @@
       </c>
     </row>
     <row r="30" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B30" s="38">
+      <c r="B30" s="32">
         <v>29</v>
       </c>
       <c r="C30" s="7" t="s">
@@ -4472,7 +4478,7 @@
       </c>
     </row>
     <row r="31" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B31" s="38">
+      <c r="B31" s="32">
         <v>30</v>
       </c>
       <c r="C31" s="7" t="s">
@@ -4489,7 +4495,7 @@
       </c>
     </row>
     <row r="32" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B32" s="38">
+      <c r="B32" s="32">
         <v>31</v>
       </c>
       <c r="C32" s="7" t="s">
@@ -4506,7 +4512,7 @@
       </c>
     </row>
     <row r="33" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B33" s="38">
+      <c r="B33" s="32">
         <v>32</v>
       </c>
       <c r="C33" s="7" t="s">
@@ -4523,7 +4529,7 @@
       </c>
     </row>
     <row r="34" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B34" s="38">
+      <c r="B34" s="32">
         <v>33</v>
       </c>
       <c r="C34" s="7" t="s">
@@ -4540,7 +4546,7 @@
       </c>
     </row>
     <row r="35" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B35" s="38">
+      <c r="B35" s="32">
         <v>34</v>
       </c>
       <c r="C35" s="7" t="s">
@@ -4557,7 +4563,7 @@
       </c>
     </row>
     <row r="36" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B36" s="38">
+      <c r="B36" s="32">
         <v>35</v>
       </c>
       <c r="C36" s="7" t="s">
@@ -4574,7 +4580,7 @@
       </c>
     </row>
     <row r="37" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B37" s="38">
+      <c r="B37" s="32">
         <v>36</v>
       </c>
       <c r="C37" s="7" t="s">
@@ -4591,7 +4597,7 @@
       </c>
     </row>
     <row r="38" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B38" s="38">
+      <c r="B38" s="32">
         <v>37</v>
       </c>
       <c r="C38" s="7" t="s">
@@ -4608,7 +4614,7 @@
       </c>
     </row>
     <row r="39" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B39" s="38">
+      <c r="B39" s="32">
         <v>38</v>
       </c>
       <c r="C39" s="7" t="s">
@@ -4625,7 +4631,7 @@
       </c>
     </row>
     <row r="40" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B40" s="38">
+      <c r="B40" s="32">
         <v>39</v>
       </c>
       <c r="C40" s="7" t="s">
@@ -4642,7 +4648,7 @@
       </c>
     </row>
     <row r="41" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B41" s="38">
+      <c r="B41" s="32">
         <v>40</v>
       </c>
       <c r="C41" s="7" t="s">
@@ -4659,7 +4665,7 @@
       </c>
     </row>
     <row r="42" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B42" s="38">
+      <c r="B42" s="32">
         <v>41</v>
       </c>
       <c r="C42" s="7" t="s">
@@ -4676,7 +4682,7 @@
       </c>
     </row>
     <row r="43" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B43" s="38">
+      <c r="B43" s="32">
         <v>42</v>
       </c>
       <c r="C43" s="7" t="s">
@@ -4693,7 +4699,7 @@
       </c>
     </row>
     <row r="44" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B44" s="38">
+      <c r="B44" s="32">
         <v>43</v>
       </c>
       <c r="C44" s="7" t="s">
@@ -4710,7 +4716,7 @@
       </c>
     </row>
     <row r="45" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B45" s="38">
+      <c r="B45" s="32">
         <v>44</v>
       </c>
       <c r="C45" s="7" t="s">
@@ -4727,7 +4733,7 @@
       </c>
     </row>
     <row r="46" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B46" s="38">
+      <c r="B46" s="32">
         <v>45</v>
       </c>
       <c r="C46" s="7" t="s">
@@ -4744,7 +4750,7 @@
       </c>
     </row>
     <row r="47" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B47" s="38">
+      <c r="B47" s="32">
         <v>46</v>
       </c>
       <c r="C47" s="7" t="s">
@@ -4761,7 +4767,7 @@
       </c>
     </row>
     <row r="48" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B48" s="38">
+      <c r="B48" s="32">
         <v>47</v>
       </c>
       <c r="C48" s="7" t="s">
@@ -4778,7 +4784,7 @@
       </c>
     </row>
     <row r="49" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B49" s="38">
+      <c r="B49" s="32">
         <v>48</v>
       </c>
       <c r="C49" s="7" t="s">
@@ -4795,7 +4801,7 @@
       </c>
     </row>
     <row r="50" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B50" s="38">
+      <c r="B50" s="32">
         <v>49</v>
       </c>
       <c r="C50" s="7" t="s">
@@ -4812,7 +4818,7 @@
       </c>
     </row>
     <row r="51" spans="2:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="B51" s="38">
+      <c r="B51" s="32">
         <v>50</v>
       </c>
       <c r="C51" s="7" t="s">
@@ -4829,7 +4835,7 @@
       </c>
     </row>
     <row r="52" spans="2:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B52" s="38">
+      <c r="B52" s="32">
         <v>51</v>
       </c>
       <c r="C52" s="7" t="s">
@@ -4846,7 +4852,7 @@
       </c>
     </row>
     <row r="53" spans="2:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B53" s="38">
+      <c r="B53" s="32">
         <v>52</v>
       </c>
       <c r="C53" s="7" t="s">
@@ -4863,7 +4869,7 @@
       </c>
     </row>
     <row r="54" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B54" s="38">
+      <c r="B54" s="32">
         <v>53</v>
       </c>
       <c r="C54" s="7" t="s">
@@ -4880,7 +4886,7 @@
       </c>
     </row>
     <row r="55" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B55" s="38">
+      <c r="B55" s="32">
         <v>54</v>
       </c>
       <c r="C55" s="7" t="s">
@@ -4897,7 +4903,7 @@
       </c>
     </row>
     <row r="56" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B56" s="38">
+      <c r="B56" s="32">
         <v>55</v>
       </c>
       <c r="C56" s="7" t="s">
@@ -4914,7 +4920,7 @@
       </c>
     </row>
     <row r="57" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B57" s="38">
+      <c r="B57" s="32">
         <v>56</v>
       </c>
       <c r="C57" s="7" t="s">
@@ -4931,7 +4937,7 @@
       </c>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B58" s="38">
+      <c r="B58" s="32">
         <v>57</v>
       </c>
       <c r="C58" s="7" t="s">
@@ -4966,10 +4972,10 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="36"/>
+      <c r="E3" s="38"/>
     </row>
     <row r="4" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D4" s="1">
@@ -4996,10 +5002,10 @@
       </c>
     </row>
     <row r="9" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D9" s="35" t="s">
+      <c r="D9" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="36"/>
+      <c r="E9" s="38"/>
     </row>
     <row r="10" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D10" s="1">
@@ -5026,10 +5032,10 @@
       </c>
     </row>
     <row r="15" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D15" s="34" t="s">
+      <c r="D15" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="34"/>
+      <c r="E15" s="36"/>
     </row>
     <row r="16" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D16" s="1" t="s">

</xml_diff>

<commit_message>
Indices estadísticos 'Nro..' de Proveedores actualizados luego de Seeds (falta hacerlo luego de buscar, contratar y calificar)
</commit_message>
<xml_diff>
--- a/Documentación/Análisis/Lista de Requerimientos - Historias de Usuarios.xlsx
+++ b/Documentación/Análisis/Lista de Requerimientos - Historias de Usuarios.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="20115" windowHeight="7995" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="20115" windowHeight="7995" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Control de versiones" sheetId="8" r:id="rId1"/>
@@ -2203,11 +2203,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2253,7 +2252,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="2" spans="2:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B2" s="31">
         <v>1</v>
       </c>
@@ -2282,7 +2281,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" ht="90" x14ac:dyDescent="0.25">
       <c r="B3" s="31">
         <v>2</v>
       </c>
@@ -2311,7 +2310,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B4" s="31">
         <v>3</v>
       </c>
@@ -2340,7 +2339,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="31">
         <v>4</v>
       </c>
@@ -2369,7 +2368,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" s="31">
         <v>5</v>
       </c>
@@ -2398,7 +2397,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B7" s="31">
         <v>6</v>
       </c>
@@ -2427,7 +2426,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B8" s="31">
         <v>7</v>
       </c>
@@ -2456,7 +2455,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B9" s="31">
         <v>8</v>
       </c>
@@ -2485,7 +2484,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B10" s="31">
         <v>9</v>
       </c>
@@ -2514,7 +2513,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="31">
         <v>10</v>
       </c>
@@ -2630,7 +2629,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" s="32">
         <v>25</v>
       </c>
@@ -2659,7 +2658,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B16" s="32">
         <v>33</v>
       </c>
@@ -2688,7 +2687,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="32">
         <v>34</v>
       </c>
@@ -2717,7 +2716,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="2:10" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B18" s="32">
         <v>35</v>
       </c>
@@ -2746,7 +2745,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="2:10" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B19" s="32">
         <v>36</v>
       </c>
@@ -2775,7 +2774,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="2:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B20" s="32">
         <v>41</v>
       </c>
@@ -2804,7 +2803,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B21" s="32">
         <v>43</v>
       </c>
@@ -2833,7 +2832,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="2:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B22" s="32">
         <v>45</v>
       </c>
@@ -2862,7 +2861,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="2:10" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B23" s="32">
         <v>46</v>
       </c>
@@ -2891,7 +2890,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="24" spans="2:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B24" s="32">
         <v>47</v>
       </c>
@@ -2920,7 +2919,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="2:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B25" s="32">
         <v>49</v>
       </c>
@@ -3007,7 +3006,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="2:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B28" s="32">
         <v>26</v>
       </c>
@@ -3036,7 +3035,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="2:10" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B29" s="32">
         <v>27</v>
       </c>
@@ -3065,7 +3064,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="2:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B30" s="32">
         <v>28</v>
       </c>
@@ -3094,7 +3093,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="2:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B31" s="32">
         <v>30</v>
       </c>
@@ -3123,7 +3122,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="32" spans="2:10" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B32" s="32">
         <v>37</v>
       </c>
@@ -3152,7 +3151,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="2:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B33" s="32">
         <v>42</v>
       </c>
@@ -3181,7 +3180,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="2:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B34" s="32">
         <v>50</v>
       </c>
@@ -3239,7 +3238,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="2:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" s="32">
         <v>53</v>
       </c>
@@ -3268,7 +3267,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="37" spans="2:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B37" s="32">
         <v>54</v>
       </c>
@@ -3297,7 +3296,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="38" spans="2:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B38" s="32">
         <v>55</v>
       </c>
@@ -3326,7 +3325,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="39" spans="2:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B39" s="32">
         <v>56</v>
       </c>
@@ -3355,7 +3354,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="40" spans="2:10" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B40" s="31">
         <v>11</v>
       </c>
@@ -3616,7 +3615,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="49" spans="2:10" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B49" s="32">
         <v>29</v>
       </c>
@@ -3645,7 +3644,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="50" spans="2:10" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:10" ht="90" x14ac:dyDescent="0.25">
       <c r="B50" s="32">
         <v>31</v>
       </c>
@@ -3674,7 +3673,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="51" spans="2:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B51" s="32">
         <v>32</v>
       </c>
@@ -3703,7 +3702,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="52" spans="2:10" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B52" s="32">
         <v>38</v>
       </c>
@@ -3732,7 +3731,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="53" spans="2:10" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B53" s="32">
         <v>39</v>
       </c>
@@ -3761,7 +3760,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="54" spans="2:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B54" s="32">
         <v>40</v>
       </c>
@@ -3790,7 +3789,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="55" spans="2:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B55" s="32">
         <v>44</v>
       </c>
@@ -3819,7 +3818,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="56" spans="2:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B56" s="32">
         <v>48</v>
       </c>
@@ -3877,7 +3876,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="58" spans="2:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B58" s="32">
         <v>57</v>
       </c>
@@ -3908,11 +3907,6 @@
     </row>
   </sheetData>
   <autoFilter ref="C1:J58">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Proveedor"/>
-      </filters>
-    </filterColumn>
     <sortState ref="C2:J58">
       <sortCondition ref="C1:C58"/>
     </sortState>
@@ -3929,8 +3923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
- Procesos de negocio actualizados - Requerimientos: algunos pintados por haberse completado - Del sistema: algunos indices 'nro..' de proveedores ya se actualizan luego de ser contratados
</commit_message>
<xml_diff>
--- a/Documentación/Análisis/Lista de Requerimientos - Historias de Usuarios.xlsx
+++ b/Documentación/Análisis/Lista de Requerimientos - Historias de Usuarios.xlsx
@@ -238,9 +238,6 @@
     <t>El sistema permitirá a los proveedores responder a las opiniones que los clientes hagan respecto de los trabajos que realicen para ellos, si es que hubieran.</t>
   </si>
   <si>
-    <t>El sistema deberá otorgar 2 leads de manera gratuita e inmediata a un nuevo proveedor cuando se registre.</t>
-  </si>
-  <si>
     <t>El sistema impedirá que los clientes, proveedores y suministradores hagan uso de las funcionalidades 2 y 4 que les corresponden y que están especificadas en las reglas de negocio, cuando sus cuentas se encuentran en estado 'Inhabilitado'.</t>
   </si>
   <si>
@@ -506,9 +503,6 @@
   </si>
   <si>
     <t>Registro y modificación de proveedores</t>
-  </si>
-  <si>
-    <t>Poder recibir 2 leads de manera gratuita e inmediata cuando me registre</t>
   </si>
   <si>
     <t>Así no tener la necesidad inmediata de ir a comprar leads</t>
@@ -1364,6 +1358,12 @@
   </si>
   <si>
     <t>El sistema deberá permitirle al cliente elegir a los proveedores luego de realizar una búsqueda manual.</t>
+  </si>
+  <si>
+    <t>Poder recibir leads de manera gratuita e inmediata cuando me registre</t>
+  </si>
+  <si>
+    <t>El sistema deberá otorgar leads de manera gratuita e inmediata a un nuevo proveedor cuando se registre. La cantidad de leads deberá poder ser configurable desde la base de datos.</t>
   </si>
 </sst>
 </file>
@@ -1434,7 +1434,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1456,6 +1456,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1587,7 +1593,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1702,6 +1708,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2044,7 +2053,7 @@
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="15"/>
       <c r="B3" s="33" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C3" s="34"/>
       <c r="D3" s="34"/>
@@ -2056,19 +2065,19 @@
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="15"/>
       <c r="B4" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="D4" s="17" t="s">
         <v>108</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>109</v>
       </c>
       <c r="E4" s="17" t="s">
         <v>16</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G4" s="18"/>
       <c r="H4" s="12"/>
@@ -2085,10 +2094,10 @@
         <v>1</v>
       </c>
       <c r="E5" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="F5" s="19" t="s">
         <v>111</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>112</v>
       </c>
       <c r="G5" s="18"/>
       <c r="H5" s="12"/>
@@ -2105,10 +2114,10 @@
         <v>2</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
@@ -2125,10 +2134,10 @@
         <v>3</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
@@ -2205,7 +2214,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
@@ -2225,7 +2234,7 @@
   <sheetData>
     <row r="1" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="31" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -2249,7 +2258,7 @@
         <v>4</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="2" spans="2:10" ht="45" x14ac:dyDescent="0.25">
@@ -2257,19 +2266,19 @@
         <v>1</v>
       </c>
       <c r="C2" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="E2" s="29" t="s">
-        <v>117</v>
-      </c>
       <c r="F2" s="5" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H2" s="27">
         <v>3</v>
@@ -2286,19 +2295,19 @@
         <v>2</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>261</v>
-      </c>
-      <c r="D3" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="D3" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>120</v>
-      </c>
-      <c r="E3" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>414</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>121</v>
       </c>
       <c r="H3" s="27">
         <v>3</v>
@@ -2315,19 +2324,19 @@
         <v>3</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>262</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>348</v>
+        <v>260</v>
+      </c>
+      <c r="D4" s="39" t="s">
+        <v>346</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="G4" s="24" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="H4" s="25">
         <v>3</v>
@@ -2344,19 +2353,19 @@
         <v>4</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>263</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>123</v>
+        <v>261</v>
+      </c>
+      <c r="D5" s="39" t="s">
+        <v>122</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="H5" s="25">
         <v>3</v>
@@ -2373,19 +2382,19 @@
         <v>5</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>264</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>124</v>
+        <v>262</v>
+      </c>
+      <c r="D6" s="39" t="s">
+        <v>123</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F6" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>330</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>332</v>
       </c>
       <c r="H6" s="25">
         <v>3</v>
@@ -2402,19 +2411,19 @@
         <v>6</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>265</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>125</v>
+        <v>263</v>
+      </c>
+      <c r="D7" s="39" t="s">
+        <v>124</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="H7" s="25">
         <v>3</v>
@@ -2431,19 +2440,19 @@
         <v>7</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>266</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>127</v>
+        <v>264</v>
+      </c>
+      <c r="D8" s="39" t="s">
+        <v>126</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H8" s="25">
         <v>3</v>
@@ -2460,19 +2469,19 @@
         <v>8</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>267</v>
-      </c>
-      <c r="D9" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="D9" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="E9" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>130</v>
-      </c>
       <c r="G9" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H9" s="25">
         <v>3</v>
@@ -2489,19 +2498,19 @@
         <v>9</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>268</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>316</v>
+        <v>266</v>
+      </c>
+      <c r="D10" s="39" t="s">
+        <v>314</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H10" s="25">
         <v>3</v>
@@ -2518,19 +2527,19 @@
         <v>10</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E11" s="29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F11" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>137</v>
       </c>
       <c r="H11" s="25">
         <v>3</v>
@@ -2547,19 +2556,19 @@
         <v>15</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E12" s="29" t="s">
         <v>10</v>
       </c>
       <c r="F12" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>141</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>142</v>
       </c>
       <c r="H12" s="25">
         <v>3</v>
@@ -2576,19 +2585,19 @@
         <v>18</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>277</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>151</v>
+        <v>275</v>
+      </c>
+      <c r="D13" s="39" t="s">
+        <v>150</v>
       </c>
       <c r="E13" s="29" t="s">
         <v>10</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H13" s="25">
         <v>3</v>
@@ -2605,19 +2614,19 @@
         <v>19</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E14" s="29" t="s">
         <v>10</v>
       </c>
       <c r="F14" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>137</v>
       </c>
       <c r="H14" s="25">
         <v>3</v>
@@ -2634,19 +2643,19 @@
         <v>25</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>284</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>171</v>
+        <v>282</v>
+      </c>
+      <c r="D15" s="39" t="s">
+        <v>169</v>
       </c>
       <c r="E15" s="29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H15" s="25">
         <v>3</v>
@@ -2655,7 +2664,7 @@
         <v>3</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="75" x14ac:dyDescent="0.25">
@@ -2663,19 +2672,19 @@
         <v>33</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>292</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>253</v>
+        <v>290</v>
+      </c>
+      <c r="D16" s="39" t="s">
+        <v>251</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="H16" s="25">
         <v>3</v>
@@ -2684,7 +2693,7 @@
         <v>2</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="30" x14ac:dyDescent="0.25">
@@ -2692,19 +2701,19 @@
         <v>34</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>293</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>189</v>
+        <v>291</v>
+      </c>
+      <c r="D17" s="39" t="s">
+        <v>187</v>
       </c>
       <c r="E17" s="29" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="H17" s="25">
         <v>3</v>
@@ -2713,7 +2722,7 @@
         <v>1</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="75" x14ac:dyDescent="0.25">
@@ -2721,19 +2730,19 @@
         <v>35</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>294</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>191</v>
+        <v>292</v>
+      </c>
+      <c r="D18" s="39" t="s">
+        <v>189</v>
       </c>
       <c r="E18" s="29" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H18" s="25">
         <v>3</v>
@@ -2742,7 +2751,7 @@
         <v>1</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="75" x14ac:dyDescent="0.25">
@@ -2750,19 +2759,19 @@
         <v>36</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>295</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>195</v>
+        <v>293</v>
+      </c>
+      <c r="D19" s="39" t="s">
+        <v>193</v>
       </c>
       <c r="E19" s="29" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="H19" s="25">
         <v>3</v>
@@ -2771,7 +2780,7 @@
         <v>1</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="60" x14ac:dyDescent="0.25">
@@ -2779,19 +2788,19 @@
         <v>41</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E20" s="29" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H20" s="25">
         <v>3</v>
@@ -2800,7 +2809,7 @@
         <v>1</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="60" x14ac:dyDescent="0.25">
@@ -2808,19 +2817,19 @@
         <v>43</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>302</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>211</v>
+        <v>300</v>
+      </c>
+      <c r="D21" s="39" t="s">
+        <v>209</v>
       </c>
       <c r="E21" s="29" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F21" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="G21" s="5" t="s">
         <v>210</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>212</v>
       </c>
       <c r="H21" s="25">
         <v>3</v>
@@ -2829,7 +2838,7 @@
         <v>2</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="60" x14ac:dyDescent="0.25">
@@ -2837,19 +2846,19 @@
         <v>45</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>304</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>258</v>
+        <v>302</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>256</v>
       </c>
       <c r="E22" s="29" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H22" s="25">
         <v>3</v>
@@ -2858,7 +2867,7 @@
         <v>2</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="2:10" ht="75" x14ac:dyDescent="0.25">
@@ -2866,19 +2875,19 @@
         <v>46</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E23" s="29" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H23" s="25">
         <v>3</v>
@@ -2887,7 +2896,7 @@
         <v>2</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="2:10" ht="60" x14ac:dyDescent="0.25">
@@ -2895,19 +2904,19 @@
         <v>47</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>306</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>222</v>
+        <v>304</v>
+      </c>
+      <c r="D24" s="39" t="s">
+        <v>220</v>
       </c>
       <c r="E24" s="29" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="H24" s="25">
         <v>3</v>
@@ -2916,7 +2925,7 @@
         <v>1</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="2:10" ht="60" x14ac:dyDescent="0.25">
@@ -2924,19 +2933,19 @@
         <v>49</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D25" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>321</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="G25" s="5" t="s">
         <v>404</v>
-      </c>
-      <c r="E25" s="29" t="s">
-        <v>323</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>405</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>406</v>
       </c>
       <c r="H25" s="25">
         <v>3</v>
@@ -2945,7 +2954,7 @@
         <v>3</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="2:10" ht="45" x14ac:dyDescent="0.25">
@@ -2953,19 +2962,19 @@
         <v>14</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E26" s="29" t="s">
         <v>10</v>
       </c>
       <c r="F26" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="G26" s="5" t="s">
         <v>133</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>134</v>
       </c>
       <c r="H26" s="25">
         <v>2</v>
@@ -2982,19 +2991,19 @@
         <v>21</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E27" s="29" t="s">
         <v>10</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="H27" s="25">
         <v>2</v>
@@ -3011,19 +3020,19 @@
         <v>26</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E28" s="29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="H28" s="25">
         <v>2</v>
@@ -3032,7 +3041,7 @@
         <v>2</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="2:10" ht="75" x14ac:dyDescent="0.25">
@@ -3040,19 +3049,19 @@
         <v>27</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H29" s="25">
         <v>2</v>
@@ -3061,7 +3070,7 @@
         <v>2</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="2:10" ht="45" x14ac:dyDescent="0.25">
@@ -3069,19 +3078,19 @@
         <v>28</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="H30" s="25">
         <v>2</v>
@@ -3090,7 +3099,7 @@
         <v>2</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="2:10" ht="30" x14ac:dyDescent="0.25">
@@ -3098,19 +3107,19 @@
         <v>30</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E31" s="29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="H31" s="25">
         <v>2</v>
@@ -3119,7 +3128,7 @@
         <v>2</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="2:10" ht="75" x14ac:dyDescent="0.25">
@@ -3127,19 +3136,19 @@
         <v>37</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E32" s="29" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H32" s="25">
         <v>2</v>
@@ -3148,7 +3157,7 @@
         <v>2</v>
       </c>
       <c r="J32" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="2:10" ht="60" x14ac:dyDescent="0.25">
@@ -3156,19 +3165,19 @@
         <v>42</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E33" s="29" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H33" s="25">
         <v>2</v>
@@ -3177,7 +3186,7 @@
         <v>2</v>
       </c>
       <c r="J33" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" spans="2:10" ht="45" x14ac:dyDescent="0.25">
@@ -3185,19 +3194,19 @@
         <v>50</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E34" s="29" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="H34" s="25">
         <v>2</v>
@@ -3206,7 +3215,7 @@
         <v>2</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="2:10" ht="45" x14ac:dyDescent="0.25">
@@ -3214,19 +3223,19 @@
         <v>51</v>
       </c>
       <c r="C35" s="25" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E35" s="29" t="s">
         <v>10</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="H35" s="25">
         <v>2</v>
@@ -3235,7 +3244,7 @@
         <v>2</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="2:10" ht="45" x14ac:dyDescent="0.25">
@@ -3243,19 +3252,19 @@
         <v>53</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E36" s="29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="H36" s="25">
         <v>2</v>
@@ -3264,7 +3273,7 @@
         <v>2</v>
       </c>
       <c r="J36" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="2:10" ht="45" x14ac:dyDescent="0.25">
@@ -3272,19 +3281,19 @@
         <v>54</v>
       </c>
       <c r="C37" s="25" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E37" s="29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="H37" s="25">
         <v>2</v>
@@ -3293,7 +3302,7 @@
         <v>2</v>
       </c>
       <c r="J37" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38" spans="2:10" ht="45" x14ac:dyDescent="0.25">
@@ -3301,19 +3310,19 @@
         <v>55</v>
       </c>
       <c r="C38" s="25" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E38" s="29" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="H38" s="25">
         <v>2</v>
@@ -3322,7 +3331,7 @@
         <v>2</v>
       </c>
       <c r="J38" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="39" spans="2:10" ht="60" x14ac:dyDescent="0.25">
@@ -3330,19 +3339,19 @@
         <v>56</v>
       </c>
       <c r="C39" s="25" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E39" s="29" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="H39" s="25">
         <v>2</v>
@@ -3351,7 +3360,7 @@
         <v>2</v>
       </c>
       <c r="J39" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="40" spans="2:10" ht="75" x14ac:dyDescent="0.25">
@@ -3359,19 +3368,19 @@
         <v>11</v>
       </c>
       <c r="C40" s="25" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E40" s="29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H40" s="25">
         <v>1</v>
@@ -3388,19 +3397,19 @@
         <v>12</v>
       </c>
       <c r="C41" s="25" t="s">
-        <v>271</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>161</v>
+        <v>269</v>
+      </c>
+      <c r="D41" s="39" t="s">
+        <v>159</v>
       </c>
       <c r="E41" s="29" t="s">
         <v>10</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H41" s="25">
         <v>1</v>
@@ -3417,19 +3426,19 @@
         <v>13</v>
       </c>
       <c r="C42" s="25" t="s">
-        <v>272</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>338</v>
+        <v>270</v>
+      </c>
+      <c r="D42" s="39" t="s">
+        <v>336</v>
       </c>
       <c r="E42" s="29" t="s">
         <v>10</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="H42" s="25">
         <v>1</v>
@@ -3446,19 +3455,19 @@
         <v>16</v>
       </c>
       <c r="C43" s="25" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E43" s="29" t="s">
         <v>10</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H43" s="25">
         <v>1</v>
@@ -3475,19 +3484,19 @@
         <v>17</v>
       </c>
       <c r="C44" s="25" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E44" s="29" t="s">
         <v>10</v>
       </c>
       <c r="F44" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="G44" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>149</v>
       </c>
       <c r="H44" s="25">
         <v>1</v>
@@ -3504,19 +3513,19 @@
         <v>20</v>
       </c>
       <c r="C45" s="25" t="s">
-        <v>279</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>156</v>
+        <v>277</v>
+      </c>
+      <c r="D45" s="39" t="s">
+        <v>154</v>
       </c>
       <c r="E45" s="29" t="s">
         <v>10</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>154</v>
+        <v>415</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H45" s="25">
         <v>1</v>
@@ -3533,19 +3542,19 @@
         <v>22</v>
       </c>
       <c r="C46" s="25" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E46" s="29" t="s">
         <v>10</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H46" s="25">
         <v>1</v>
@@ -3562,19 +3571,19 @@
         <v>23</v>
       </c>
       <c r="C47" s="25" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E47" s="29" t="s">
         <v>10</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H47" s="25">
         <v>1</v>
@@ -3591,19 +3600,19 @@
         <v>24</v>
       </c>
       <c r="C48" s="25" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E48" s="29" t="s">
         <v>10</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H48" s="25">
         <v>1</v>
@@ -3612,7 +3621,7 @@
         <v>2</v>
       </c>
       <c r="J48" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="49" spans="2:10" ht="75" x14ac:dyDescent="0.25">
@@ -3620,19 +3629,19 @@
         <v>29</v>
       </c>
       <c r="C49" s="25" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E49" s="29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H49" s="25">
         <v>1</v>
@@ -3641,7 +3650,7 @@
         <v>3</v>
       </c>
       <c r="J49" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="50" spans="2:10" ht="90" x14ac:dyDescent="0.25">
@@ -3649,19 +3658,19 @@
         <v>31</v>
       </c>
       <c r="C50" s="25" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E50" s="29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H50" s="25">
         <v>1</v>
@@ -3670,7 +3679,7 @@
         <v>3</v>
       </c>
       <c r="J50" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="51" spans="2:10" ht="60" x14ac:dyDescent="0.25">
@@ -3678,19 +3687,19 @@
         <v>32</v>
       </c>
       <c r="C51" s="25" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E51" s="29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F51" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="G51" s="5" t="s">
         <v>244</v>
-      </c>
-      <c r="G51" s="5" t="s">
-        <v>246</v>
       </c>
       <c r="H51" s="25">
         <v>1</v>
@@ -3699,7 +3708,7 @@
         <v>3</v>
       </c>
       <c r="J51" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="52" spans="2:10" ht="75" x14ac:dyDescent="0.25">
@@ -3707,19 +3716,19 @@
         <v>38</v>
       </c>
       <c r="C52" s="25" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E52" s="29" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H52" s="25">
         <v>1</v>
@@ -3728,7 +3737,7 @@
         <v>1</v>
       </c>
       <c r="J52" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="53" spans="2:10" ht="75" x14ac:dyDescent="0.25">
@@ -3736,19 +3745,19 @@
         <v>39</v>
       </c>
       <c r="C53" s="25" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D53" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="E53" s="29" t="s">
         <v>321</v>
       </c>
-      <c r="E53" s="29" t="s">
-        <v>323</v>
-      </c>
       <c r="F53" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H53" s="25">
         <v>1</v>
@@ -3757,7 +3766,7 @@
         <v>2</v>
       </c>
       <c r="J53" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="54" spans="2:10" ht="60" x14ac:dyDescent="0.25">
@@ -3765,19 +3774,19 @@
         <v>40</v>
       </c>
       <c r="C54" s="25" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E54" s="29" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H54" s="25">
         <v>1</v>
@@ -3786,7 +3795,7 @@
         <v>3</v>
       </c>
       <c r="J54" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="55" spans="2:10" ht="30" x14ac:dyDescent="0.25">
@@ -3794,19 +3803,19 @@
         <v>44</v>
       </c>
       <c r="C55" s="25" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E55" s="29" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F55" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="G55" s="5" t="s">
         <v>213</v>
-      </c>
-      <c r="G55" s="5" t="s">
-        <v>215</v>
       </c>
       <c r="H55" s="25">
         <v>1</v>
@@ -3815,7 +3824,7 @@
         <v>1</v>
       </c>
       <c r="J55" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="56" spans="2:10" ht="45" x14ac:dyDescent="0.25">
@@ -3823,19 +3832,19 @@
         <v>48</v>
       </c>
       <c r="C56" s="25" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E56" s="29" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="H56" s="25">
         <v>1</v>
@@ -3844,7 +3853,7 @@
         <v>1</v>
       </c>
       <c r="J56" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="57" spans="2:10" ht="90" x14ac:dyDescent="0.25">
@@ -3852,19 +3861,19 @@
         <v>52</v>
       </c>
       <c r="C57" s="25" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E57" s="29" t="s">
         <v>10</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="H57" s="25">
         <v>1</v>
@@ -3873,7 +3882,7 @@
         <v>3</v>
       </c>
       <c r="J57" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="58" spans="2:10" ht="45" x14ac:dyDescent="0.25">
@@ -3881,19 +3890,19 @@
         <v>57</v>
       </c>
       <c r="C58" s="25" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E58" s="29" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F58" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="G58" s="5" t="s">
         <v>247</v>
-      </c>
-      <c r="G58" s="5" t="s">
-        <v>249</v>
       </c>
       <c r="H58" s="25">
         <v>1</v>
@@ -3902,7 +3911,7 @@
         <v>3</v>
       </c>
       <c r="J58" s="7" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
   </sheetData>
@@ -3923,8 +3932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I58"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3942,13 +3951,13 @@
   <sheetData>
     <row r="1" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="31" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>40</v>
@@ -3965,7 +3974,7 @@
         <v>17</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>45</v>
@@ -3974,7 +3983,7 @@
         <v>12</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I2" s="9">
         <f>COUNTIF(F2:F58,"E")</f>
@@ -3998,7 +4007,7 @@
         <v>12</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I3" s="9">
         <f>COUNTIF(F2:F58,"D")</f>
@@ -4013,7 +4022,7 @@
         <v>19</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>45</v>
@@ -4022,7 +4031,7 @@
         <v>12</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I4" s="11">
         <f>SUM(I2:I3)</f>
@@ -4037,7 +4046,7 @@
         <v>20</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>45</v>
@@ -4054,7 +4063,7 @@
         <v>21</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>45</v>
@@ -4071,7 +4080,7 @@
         <v>22</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>45</v>
@@ -4156,7 +4165,7 @@
         <v>27</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>45</v>
@@ -4190,7 +4199,7 @@
         <v>29</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>41</v>
@@ -4207,7 +4216,7 @@
         <v>30</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>41</v>
@@ -4301,7 +4310,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B21" s="32">
         <v>20</v>
       </c>
@@ -4309,7 +4318,7 @@
         <v>36</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>64</v>
+        <v>416</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>41</v>
@@ -4374,10 +4383,10 @@
         <v>24</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D25" s="22" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>41</v>
@@ -4391,10 +4400,10 @@
         <v>25</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>42</v>
@@ -4408,10 +4417,10 @@
         <v>26</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>42</v>
@@ -4425,10 +4434,10 @@
         <v>27</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>42</v>
@@ -4442,10 +4451,10 @@
         <v>28</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>42</v>
@@ -4459,10 +4468,10 @@
         <v>29</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D30" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>42</v>
@@ -4476,10 +4485,10 @@
         <v>30</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D31" s="22" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>42</v>
@@ -4493,10 +4502,10 @@
         <v>31</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D32" s="22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>42</v>
@@ -4510,10 +4519,10 @@
         <v>32</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D33" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>42</v>
@@ -4527,10 +4536,10 @@
         <v>33</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D34" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>43</v>
@@ -4544,10 +4553,10 @@
         <v>34</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>43</v>
@@ -4561,10 +4570,10 @@
         <v>35</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>43</v>
@@ -4578,7 +4587,7 @@
         <v>36</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D37" s="22" t="s">
         <v>47</v>
@@ -4595,10 +4604,10 @@
         <v>37</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D38" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>43</v>
@@ -4612,10 +4621,10 @@
         <v>38</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>43</v>
@@ -4629,10 +4638,10 @@
         <v>39</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D40" s="22" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>43</v>
@@ -4646,10 +4655,10 @@
         <v>40</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D41" s="22" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>43</v>
@@ -4663,7 +4672,7 @@
         <v>41</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D42" s="22" t="s">
         <v>58</v>
@@ -4680,10 +4689,10 @@
         <v>42</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D43" s="22" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>43</v>
@@ -4697,7 +4706,7 @@
         <v>43</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D44" s="22" t="s">
         <v>44</v>
@@ -4714,10 +4723,10 @@
         <v>44</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D45" s="22" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>43</v>
@@ -4731,7 +4740,7 @@
         <v>45</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D46" s="22" t="s">
         <v>59</v>
@@ -4748,10 +4757,10 @@
         <v>46</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D47" s="22" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>43</v>
@@ -4765,7 +4774,7 @@
         <v>47</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D48" s="22" t="s">
         <v>60</v>
@@ -4782,10 +4791,10 @@
         <v>48</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D49" s="22" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>43</v>
@@ -4799,10 +4808,10 @@
         <v>49</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D50" s="22" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>43</v>
@@ -4816,13 +4825,13 @@
         <v>50</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D51" s="22" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F51" s="7" t="s">
         <v>12</v>
@@ -4833,13 +4842,13 @@
         <v>51</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D52" s="22" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F52" s="7" t="s">
         <v>12</v>
@@ -4850,13 +4859,13 @@
         <v>52</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D53" s="22" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F53" s="7" t="s">
         <v>13</v>
@@ -4867,13 +4876,13 @@
         <v>53</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D54" s="22" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F54" s="7" t="s">
         <v>12</v>
@@ -4884,13 +4893,13 @@
         <v>54</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D55" s="22" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F55" s="7" t="s">
         <v>12</v>
@@ -4901,13 +4910,13 @@
         <v>55</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D56" s="22" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F56" s="7" t="s">
         <v>12</v>
@@ -4918,13 +4927,13 @@
         <v>56</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D57" s="22" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F57" s="7" t="s">
         <v>12</v>
@@ -4935,13 +4944,13 @@
         <v>57</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D58" s="22" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F58" s="7" t="s">
         <v>13</v>
@@ -5078,7 +5087,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>11</v>
@@ -5086,10 +5095,10 @@
     </row>
     <row r="2" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C2" s="7" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>12</v>
@@ -5097,10 +5106,10 @@
     </row>
     <row r="3" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C3" s="7" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>12</v>
@@ -5108,10 +5117,10 @@
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C4" s="7" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>12</v>
@@ -5119,10 +5128,10 @@
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C5" s="7" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>13</v>
@@ -5130,10 +5139,10 @@
     </row>
     <row r="6" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C6" s="7" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>12</v>
@@ -5141,10 +5150,10 @@
     </row>
     <row r="7" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C7" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>13</v>
@@ -5152,10 +5161,10 @@
     </row>
     <row r="8" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C8" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>13</v>
@@ -5163,10 +5172,10 @@
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C9" s="7" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>13</v>
@@ -5174,10 +5183,10 @@
     </row>
     <row r="10" spans="3:5" ht="60" x14ac:dyDescent="0.25">
       <c r="C10" s="7" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>13</v>
@@ -5185,10 +5194,10 @@
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C11" s="7" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>13</v>
@@ -5196,10 +5205,10 @@
     </row>
     <row r="12" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C12" s="7" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>12</v>
@@ -5207,10 +5216,10 @@
     </row>
     <row r="13" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C13" s="7" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>13</v>
@@ -5218,10 +5227,10 @@
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C14" s="7" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>13</v>
@@ -5229,10 +5238,10 @@
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C15" s="7" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>12</v>
@@ -5240,10 +5249,10 @@
     </row>
     <row r="16" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C16" s="7" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>13</v>
@@ -5251,10 +5260,10 @@
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C17" s="7" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>13</v>
@@ -5262,10 +5271,10 @@
     </row>
     <row r="18" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C18" s="7" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>13</v>
@@ -5273,10 +5282,10 @@
     </row>
     <row r="19" spans="3:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C19" s="7" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>13</v>
@@ -5284,10 +5293,10 @@
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C20" s="7" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
DOCUMENTO DE TESIS CON FORMATO - CAP8: ANALISIS
</commit_message>
<xml_diff>
--- a/Documentación/Análisis/Lista de Requerimientos - Historias de Usuarios.xlsx
+++ b/Documentación/Análisis/Lista de Requerimientos - Historias de Usuarios.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="20115" windowHeight="7995" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="20115" windowHeight="7995" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Control de versiones" sheetId="8" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="426">
   <si>
     <t>ID</t>
   </si>
@@ -1365,12 +1365,39 @@
   <si>
     <t>El sistema deberá otorgar leads de manera gratuita e inmediata a un nuevo proveedor cuando se registre. La cantidad de leads deberá poder ser configurable desde la base de datos.</t>
   </si>
+  <si>
+    <t>PRIORIDAD</t>
+  </si>
+  <si>
+    <t>DIFICULTAD</t>
+  </si>
+  <si>
+    <t>EXIGIBILIDAD</t>
+  </si>
+  <si>
+    <t>TIPO DE PERFIL</t>
+  </si>
+  <si>
+    <t>DESCRIPCIÓN DEL PERFIL</t>
+  </si>
+  <si>
+    <t>Tiendas, cadenas y personas jurídicas que estén en el rubro de la venta de materiales para construcción, remodelamiento, mantenimiento, y cualquier otro objeto relacionado (también conocidas como ferreterías)</t>
+  </si>
+  <si>
+    <t>Persona que tiene habilitados todos los permisos de edición de código y acceso a la información de las bases de datos ya sea para dar mantenimiento, soporte, actualización, entre otros</t>
+  </si>
+  <si>
+    <t>Toda persona natural o jurídica que brinde uno o más de los servicios generales considerados en el presente proyecto.</t>
+  </si>
+  <si>
+    <t>Toda persona natural o jurídica que tenga intenciones de contratar cualquiera de los servicios generales considerados en el presente proyecto</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1432,6 +1459,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1593,7 +1626,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1691,6 +1724,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1709,7 +1748,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2052,13 +2094,13 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="15"/>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="35"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="37"/>
       <c r="G3" s="16"/>
       <c r="H3" s="12"/>
     </row>
@@ -2214,7 +2256,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
@@ -2268,7 +2310,7 @@
       <c r="C2" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="34" t="s">
         <v>118</v>
       </c>
       <c r="E2" s="29" t="s">
@@ -2297,7 +2339,7 @@
       <c r="C3" s="25" t="s">
         <v>259</v>
       </c>
-      <c r="D3" s="39" t="s">
+      <c r="D3" s="34" t="s">
         <v>119</v>
       </c>
       <c r="E3" s="29" t="s">
@@ -2326,7 +2368,7 @@
       <c r="C4" s="25" t="s">
         <v>260</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="34" t="s">
         <v>346</v>
       </c>
       <c r="E4" s="29" t="s">
@@ -2355,7 +2397,7 @@
       <c r="C5" s="25" t="s">
         <v>261</v>
       </c>
-      <c r="D5" s="39" t="s">
+      <c r="D5" s="34" t="s">
         <v>122</v>
       </c>
       <c r="E5" s="29" t="s">
@@ -2384,7 +2426,7 @@
       <c r="C6" s="25" t="s">
         <v>262</v>
       </c>
-      <c r="D6" s="39" t="s">
+      <c r="D6" s="34" t="s">
         <v>123</v>
       </c>
       <c r="E6" s="29" t="s">
@@ -2413,7 +2455,7 @@
       <c r="C7" s="25" t="s">
         <v>263</v>
       </c>
-      <c r="D7" s="39" t="s">
+      <c r="D7" s="34" t="s">
         <v>124</v>
       </c>
       <c r="E7" s="29" t="s">
@@ -2442,7 +2484,7 @@
       <c r="C8" s="25" t="s">
         <v>264</v>
       </c>
-      <c r="D8" s="39" t="s">
+      <c r="D8" s="34" t="s">
         <v>126</v>
       </c>
       <c r="E8" s="29" t="s">
@@ -2471,7 +2513,7 @@
       <c r="C9" s="25" t="s">
         <v>265</v>
       </c>
-      <c r="D9" s="39" t="s">
+      <c r="D9" s="34" t="s">
         <v>128</v>
       </c>
       <c r="E9" s="29" t="s">
@@ -2500,7 +2542,7 @@
       <c r="C10" s="25" t="s">
         <v>266</v>
       </c>
-      <c r="D10" s="39" t="s">
+      <c r="D10" s="34" t="s">
         <v>314</v>
       </c>
       <c r="E10" s="29" t="s">
@@ -2587,7 +2629,7 @@
       <c r="C13" s="25" t="s">
         <v>275</v>
       </c>
-      <c r="D13" s="39" t="s">
+      <c r="D13" s="34" t="s">
         <v>150</v>
       </c>
       <c r="E13" s="29" t="s">
@@ -2645,7 +2687,7 @@
       <c r="C15" s="25" t="s">
         <v>282</v>
       </c>
-      <c r="D15" s="39" t="s">
+      <c r="D15" s="34" t="s">
         <v>169</v>
       </c>
       <c r="E15" s="29" t="s">
@@ -2674,7 +2716,7 @@
       <c r="C16" s="25" t="s">
         <v>290</v>
       </c>
-      <c r="D16" s="39" t="s">
+      <c r="D16" s="34" t="s">
         <v>251</v>
       </c>
       <c r="E16" s="29" t="s">
@@ -2703,7 +2745,7 @@
       <c r="C17" s="25" t="s">
         <v>291</v>
       </c>
-      <c r="D17" s="39" t="s">
+      <c r="D17" s="34" t="s">
         <v>187</v>
       </c>
       <c r="E17" s="29" t="s">
@@ -2732,7 +2774,7 @@
       <c r="C18" s="25" t="s">
         <v>292</v>
       </c>
-      <c r="D18" s="39" t="s">
+      <c r="D18" s="34" t="s">
         <v>189</v>
       </c>
       <c r="E18" s="29" t="s">
@@ -2761,7 +2803,7 @@
       <c r="C19" s="25" t="s">
         <v>293</v>
       </c>
-      <c r="D19" s="39" t="s">
+      <c r="D19" s="34" t="s">
         <v>193</v>
       </c>
       <c r="E19" s="29" t="s">
@@ -2819,7 +2861,7 @@
       <c r="C21" s="25" t="s">
         <v>300</v>
       </c>
-      <c r="D21" s="39" t="s">
+      <c r="D21" s="34" t="s">
         <v>209</v>
       </c>
       <c r="E21" s="29" t="s">
@@ -2906,7 +2948,7 @@
       <c r="C24" s="25" t="s">
         <v>304</v>
       </c>
-      <c r="D24" s="39" t="s">
+      <c r="D24" s="34" t="s">
         <v>220</v>
       </c>
       <c r="E24" s="29" t="s">
@@ -3399,7 +3441,7 @@
       <c r="C41" s="25" t="s">
         <v>269</v>
       </c>
-      <c r="D41" s="39" t="s">
+      <c r="D41" s="34" t="s">
         <v>159</v>
       </c>
       <c r="E41" s="29" t="s">
@@ -3428,7 +3470,7 @@
       <c r="C42" s="25" t="s">
         <v>270</v>
       </c>
-      <c r="D42" s="39" t="s">
+      <c r="D42" s="34" t="s">
         <v>336</v>
       </c>
       <c r="E42" s="29" t="s">
@@ -3515,7 +3557,7 @@
       <c r="C45" s="25" t="s">
         <v>277</v>
       </c>
-      <c r="D45" s="39" t="s">
+      <c r="D45" s="34" t="s">
         <v>154</v>
       </c>
       <c r="E45" s="29" t="s">
@@ -3932,7 +3974,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I58"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -4966,19 +5008,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D3:E17"/>
+  <dimension ref="D3:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19:H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="55.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="3" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D3" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="38"/>
+      <c r="D3" s="39" t="s">
+        <v>417</v>
+      </c>
+      <c r="E3" s="40"/>
     </row>
     <row r="4" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D4" s="1">
@@ -5005,10 +5051,10 @@
       </c>
     </row>
     <row r="9" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D9" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" s="38"/>
+      <c r="D9" s="39" t="s">
+        <v>418</v>
+      </c>
+      <c r="E9" s="40"/>
     </row>
     <row r="10" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D10" s="1">
@@ -5035,10 +5081,10 @@
       </c>
     </row>
     <row r="15" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D15" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="36"/>
+      <c r="D15" s="38" t="s">
+        <v>419</v>
+      </c>
+      <c r="E15" s="38"/>
     </row>
     <row r="16" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D16" s="1" t="s">
@@ -5048,12 +5094,52 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="G19" s="33" t="s">
+        <v>420</v>
+      </c>
+      <c r="H19" s="33" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="20" spans="4:8" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="G20" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H20" s="41" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="21" spans="4:8" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="G21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" s="42" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="22" spans="4:8" ht="43.5" x14ac:dyDescent="0.25">
+      <c r="G22" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H22" s="41" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="23" spans="4:8" ht="43.5" x14ac:dyDescent="0.25">
+      <c r="G23" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="H23" s="41" t="s">
+        <v>423</v>
       </c>
     </row>
   </sheetData>
@@ -5063,6 +5149,7 @@
     <mergeCell ref="D3:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5070,7 +5157,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:E20"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Visualizar Ofertas, Promos y Dsctos 100% Separa una oferta, promo, dscto 0%
</commit_message>
<xml_diff>
--- a/Documentación/Análisis/Lista de Requerimientos - Historias de Usuarios.xlsx
+++ b/Documentación/Análisis/Lista de Requerimientos - Historias de Usuarios.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="18840" windowHeight="7725" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="18840" windowHeight="7725" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Control de versiones" sheetId="8" r:id="rId1"/>
@@ -2256,8 +2256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3974,8 +3974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I58"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
CSS Datepicker Registros Imagenes en registros Registrarme Otros cambios menores
</commit_message>
<xml_diff>
--- a/Documentación/Análisis/Lista de Requerimientos - Historias de Usuarios.xlsx
+++ b/Documentación/Análisis/Lista de Requerimientos - Historias de Usuarios.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="18840" windowHeight="7725" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="18840" windowHeight="7725" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Control de versiones" sheetId="8" r:id="rId1"/>
@@ -2256,7 +2256,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
@@ -3035,7 +3035,7 @@
       <c r="C27" s="25" t="s">
         <v>278</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="34" t="s">
         <v>156</v>
       </c>
       <c r="E27" s="29" t="s">
@@ -3093,7 +3093,7 @@
       <c r="C29" s="25" t="s">
         <v>284</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="34" t="s">
         <v>172</v>
       </c>
       <c r="E29" s="29" t="s">
@@ -3974,8 +3974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Documento revisado por Aguilera EditarMiInformacion
</commit_message>
<xml_diff>
--- a/Documentación/Análisis/Lista de Requerimientos - Historias de Usuarios.xlsx
+++ b/Documentación/Análisis/Lista de Requerimientos - Historias de Usuarios.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="18840" windowHeight="7725" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="18840" windowHeight="7725" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Control de versiones" sheetId="8" r:id="rId1"/>
@@ -1733,6 +1733,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1751,10 +1755,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2095,13 +2095,13 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="15"/>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="38"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="40"/>
       <c r="G3" s="16"/>
       <c r="H3" s="12"/>
     </row>
@@ -2257,7 +2257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
       <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
@@ -5022,10 +5022,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="42" t="s">
         <v>400</v>
       </c>
-      <c r="E3" s="41"/>
+      <c r="E3" s="43"/>
     </row>
     <row r="4" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D4" s="1">
@@ -5052,10 +5052,10 @@
       </c>
     </row>
     <row r="9" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D9" s="40" t="s">
+      <c r="D9" s="42" t="s">
         <v>401</v>
       </c>
-      <c r="E9" s="41"/>
+      <c r="E9" s="43"/>
     </row>
     <row r="10" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D10" s="1">
@@ -5082,10 +5082,10 @@
       </c>
     </row>
     <row r="15" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D15" s="39" t="s">
+      <c r="D15" s="41" t="s">
         <v>402</v>
       </c>
-      <c r="E15" s="39"/>
+      <c r="E15" s="41"/>
     </row>
     <row r="16" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D16" s="1" t="s">
@@ -5158,7 +5158,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -5391,10 +5391,10 @@
       </c>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C21" s="42" t="s">
+      <c r="C21" s="36" t="s">
         <v>426</v>
       </c>
-      <c r="D21" s="43" t="s">
+      <c r="D21" s="37" t="s">
         <v>427</v>
       </c>
       <c r="E21" s="7" t="s">

</xml_diff>

<commit_message>
Reporte Consolidado Historico Trabajos
</commit_message>
<xml_diff>
--- a/Documentación/Análisis/Lista de Requerimientos - Historias de Usuarios.xlsx
+++ b/Documentación/Análisis/Lista de Requerimientos - Historias de Usuarios.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="18840" windowHeight="7725" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="18840" windowHeight="7725" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Control de versiones" sheetId="8" r:id="rId1"/>
@@ -1120,18 +1120,12 @@
     <t>Versión 3</t>
   </si>
   <si>
-    <t>El sistema deberá permitirle al proveedor generar un reporte (en formato de tabla) de todos los trabajos pendientes y realizados por éste, con el detalle del nro. de recibo por honorarios/factura (si hubiera), tipo de servicio, cliente, fecha, dirección, descripción corta, calificación, y monto cobrado, para un rango de fechas dadas.</t>
-  </si>
-  <si>
     <t>El sistema deberá permitirle al administrador generar un reporte (en formato de tabla) del histórico de todos los trabajos realizados, con el detalle del nro. de recibo por honorarios/factura (si hubiera), tipo de servicio, proveedor, cliente, fecha, dirección, descripción corta, calificación, y monto cobrado, para un rango de fechas dadas.</t>
   </si>
   <si>
     <t>El sistema deberá permitirle al suministrador generar un reporte (en formato de tabla) de demanda de búsqueda y visita a productos (clicks por búsqueda y acceso).</t>
   </si>
   <si>
-    <t>El sistema deberá permitirle a los proveedores y suministradores generar un reporte (en formato de tabla) de demanda de servicios, clasificado por distritos, tipos de servicios, y demanda, para un rango de fechas dadas.</t>
-  </si>
-  <si>
     <t>Así poder visualizar todos los trabajos que alguna vez se han realizado</t>
   </si>
   <si>
@@ -1397,6 +1391,12 @@
   </si>
   <si>
     <t>El sistema deberá hacer uso de Captcha para evitar bots en el registro de usuarios</t>
+  </si>
+  <si>
+    <t>El sistema deberá permitirle al proveedor generar un reporte consolidado (en formato de tabla) de todos los trabajos realizados por éste, con el detalle del nro. de recibo por honorarios/factura (si hubiera), tipo de servicio, cliente, fecha, dirección, descripción corta, calificación, y monto cobrado, para un rango de fechas dadas.</t>
+  </si>
+  <si>
+    <t>El sistema deberá permitirle a los proveedores generar un reporte (en formato de tabla) de demanda de servicios generales, clasificado por distritos, tipos de servicios, y demanda, para un rango de fechas dadas.</t>
   </si>
 </sst>
 </file>
@@ -1473,7 +1473,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1495,6 +1495,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1626,7 +1632,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1754,6 +1760,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2257,8 +2266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2277,7 +2286,7 @@
   <sheetData>
     <row r="1" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="30" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -2318,7 +2327,7 @@
         <v>114</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>119</v>
@@ -2347,7 +2356,7 @@
         <v>114</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>118</v>
@@ -2376,7 +2385,7 @@
         <v>114</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="G4" s="24" t="s">
         <v>317</v>
@@ -2408,7 +2417,7 @@
         <v>313</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="H5" s="25">
         <v>3</v>
@@ -2463,7 +2472,7 @@
         <v>114</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>315</v>
@@ -2611,7 +2620,7 @@
         <v>138</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="H12" s="25">
         <v>3</v>
@@ -2979,16 +2988,16 @@
         <v>293</v>
       </c>
       <c r="D25" s="33" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E25" s="28" t="s">
         <v>308</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="H25" s="25">
         <v>3</v>
@@ -3066,16 +3075,16 @@
         <v>270</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E28" s="28" t="s">
         <v>115</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="H28" s="25">
         <v>2</v>
@@ -3095,16 +3104,16 @@
         <v>271</v>
       </c>
       <c r="D29" s="33" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E29" s="28" t="s">
         <v>115</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="H29" s="25">
         <v>2</v>
@@ -3124,16 +3133,16 @@
         <v>272</v>
       </c>
       <c r="D30" s="33" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="E30" s="28" t="s">
         <v>115</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="H30" s="25">
         <v>2</v>
@@ -3249,7 +3258,7 @@
         <v>216</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="H34" s="25">
         <v>2</v>
@@ -3385,16 +3394,16 @@
         <v>322</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E39" s="28" t="s">
         <v>308</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="H39" s="25">
         <v>2</v>
@@ -3565,7 +3574,7 @@
         <v>10</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>150</v>
@@ -3675,7 +3684,7 @@
         <v>273</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="E49" s="28" t="s">
         <v>115</v>
@@ -3916,7 +3925,7 @@
         <v>220</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="H57" s="25">
         <v>1</v>
@@ -3933,7 +3942,7 @@
         <v>57</v>
       </c>
       <c r="C58" s="25" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D58" s="5" t="s">
         <v>238</v>
@@ -3954,7 +3963,7 @@
         <v>3</v>
       </c>
       <c r="J58" s="7" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
   </sheetData>
@@ -3975,8 +3984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I58"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView tabSelected="1" topLeftCell="B51" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51:D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3994,7 +4003,7 @@
   <sheetData>
     <row r="1" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="30" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
@@ -4065,7 +4074,7 @@
         <v>19</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>45</v>
@@ -4123,7 +4132,7 @@
         <v>22</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>45</v>
@@ -4259,7 +4268,7 @@
         <v>30</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>41</v>
@@ -4361,7 +4370,7 @@
         <v>36</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>41</v>
@@ -4378,7 +4387,7 @@
         <v>37</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>41</v>
@@ -4463,7 +4472,7 @@
         <v>75</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>42</v>
@@ -4480,7 +4489,7 @@
         <v>76</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>42</v>
@@ -4497,7 +4506,7 @@
         <v>77</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>42</v>
@@ -4616,7 +4625,7 @@
         <v>84</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>43</v>
@@ -4837,7 +4846,7 @@
         <v>97</v>
       </c>
       <c r="D49" s="22" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>43</v>
@@ -4854,7 +4863,7 @@
         <v>98</v>
       </c>
       <c r="D50" s="22" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>43</v>
@@ -4870,8 +4879,8 @@
       <c r="C51" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="D51" s="22" t="s">
-        <v>336</v>
+      <c r="D51" s="44" t="s">
+        <v>335</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>68</v>
@@ -4887,8 +4896,8 @@
       <c r="C52" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="D52" s="22" t="s">
-        <v>335</v>
+      <c r="D52" s="44" t="s">
+        <v>426</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>68</v>
@@ -4921,8 +4930,8 @@
       <c r="C54" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D54" s="22" t="s">
-        <v>425</v>
+      <c r="D54" s="44" t="s">
+        <v>423</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>68</v>
@@ -4938,8 +4947,8 @@
       <c r="C55" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="D55" s="22" t="s">
-        <v>337</v>
+      <c r="D55" s="44" t="s">
+        <v>336</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>68</v>
@@ -4955,7 +4964,7 @@
       <c r="C56" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="D56" s="22" t="s">
+      <c r="D56" s="44" t="s">
         <v>333</v>
       </c>
       <c r="E56" s="2" t="s">
@@ -4972,8 +4981,8 @@
       <c r="C57" s="7" t="s">
         <v>323</v>
       </c>
-      <c r="D57" s="22" t="s">
-        <v>338</v>
+      <c r="D57" s="44" t="s">
+        <v>427</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>68</v>
@@ -4987,7 +4996,7 @@
         <v>57</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D58" s="22" t="s">
         <v>236</v>
@@ -5023,7 +5032,7 @@
   <sheetData>
     <row r="3" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D3" s="42" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="E3" s="43"/>
     </row>
@@ -5053,7 +5062,7 @@
     </row>
     <row r="9" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D9" s="42" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E9" s="43"/>
     </row>
@@ -5083,7 +5092,7 @@
     </row>
     <row r="15" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D15" s="41" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="E15" s="41"/>
     </row>
@@ -5105,10 +5114,10 @@
     </row>
     <row r="19" spans="4:8" x14ac:dyDescent="0.25">
       <c r="G19" s="32" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="H19" s="32" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="20" spans="4:8" ht="43.5" x14ac:dyDescent="0.25">
@@ -5116,7 +5125,7 @@
         <v>114</v>
       </c>
       <c r="H20" s="34" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="21" spans="4:8" ht="42.75" x14ac:dyDescent="0.25">
@@ -5124,7 +5133,7 @@
         <v>10</v>
       </c>
       <c r="H21" s="35" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="22" spans="4:8" ht="57.75" x14ac:dyDescent="0.25">
@@ -5132,7 +5141,7 @@
         <v>115</v>
       </c>
       <c r="H22" s="34" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="23" spans="4:8" ht="57.75" x14ac:dyDescent="0.25">
@@ -5140,7 +5149,7 @@
         <v>308</v>
       </c>
       <c r="H23" s="34" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
   </sheetData>
@@ -5183,10 +5192,10 @@
     </row>
     <row r="2" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C2" s="7" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>12</v>
@@ -5194,10 +5203,10 @@
     </row>
     <row r="3" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C3" s="7" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>12</v>
@@ -5205,10 +5214,10 @@
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C4" s="7" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>12</v>
@@ -5216,10 +5225,10 @@
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C5" s="7" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>13</v>
@@ -5227,10 +5236,10 @@
     </row>
     <row r="6" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C6" s="7" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>12</v>
@@ -5238,10 +5247,10 @@
     </row>
     <row r="7" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C7" s="7" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>13</v>
@@ -5249,10 +5258,10 @@
     </row>
     <row r="8" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C8" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>13</v>
@@ -5260,10 +5269,10 @@
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C9" s="7" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>13</v>
@@ -5271,10 +5280,10 @@
     </row>
     <row r="10" spans="3:5" ht="60" x14ac:dyDescent="0.25">
       <c r="C10" s="7" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>13</v>
@@ -5282,10 +5291,10 @@
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C11" s="7" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>13</v>
@@ -5293,10 +5302,10 @@
     </row>
     <row r="12" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C12" s="7" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>12</v>
@@ -5304,10 +5313,10 @@
     </row>
     <row r="13" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C13" s="7" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>13</v>
@@ -5315,10 +5324,10 @@
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C14" s="7" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>13</v>
@@ -5326,10 +5335,10 @@
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C15" s="7" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>12</v>
@@ -5337,10 +5346,10 @@
     </row>
     <row r="16" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C16" s="7" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>13</v>
@@ -5348,10 +5357,10 @@
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C17" s="7" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>13</v>
@@ -5359,10 +5368,10 @@
     </row>
     <row r="18" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C18" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>13</v>
@@ -5370,10 +5379,10 @@
     </row>
     <row r="19" spans="3:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C19" s="7" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>13</v>
@@ -5381,10 +5390,10 @@
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C20" s="7" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>13</v>
@@ -5392,10 +5401,10 @@
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C21" s="36" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="D21" s="37" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Reporte Demanda de ofertas, promociones y descuentos
</commit_message>
<xml_diff>
--- a/Documentación/Análisis/Lista de Requerimientos - Historias de Usuarios.xlsx
+++ b/Documentación/Análisis/Lista de Requerimientos - Historias de Usuarios.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="18840" windowHeight="7725" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="18840" windowHeight="7725" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Control de versiones" sheetId="8" r:id="rId1"/>
@@ -1384,19 +1384,19 @@
     <t>El sistema deberá permitir que los proveedores puedan cambiar sus leads para adquirir ofertas, promociones y descuentos en tiendas y cadenas suministradoras (compra virtual).</t>
   </si>
   <si>
-    <t>El sistema deberá permitirle al suministrador generar un reporte (en formato de tabla) con las ofertas, promociones y descuentos más vendidos, para un rango de fechas dadas.</t>
-  </si>
-  <si>
     <t>R77</t>
   </si>
   <si>
     <t>El sistema deberá hacer uso de Captcha para evitar bots en el registro de usuarios</t>
   </si>
   <si>
-    <t>El sistema deberá permitirle al proveedor generar un reporte consolidado (en formato de tabla) de todos los trabajos realizados por éste, con el detalle del nro. de recibo por honorarios/factura (si hubiera), tipo de servicio, cliente, fecha, dirección, descripción corta, calificación, y monto cobrado, para un rango de fechas dadas.</t>
-  </si>
-  <si>
     <t>El sistema deberá permitirle a los proveedores generar un reporte (en formato de tabla) de demanda de servicios generales, clasificado por distritos, tipos de servicios, y demanda, para un rango de fechas dadas.</t>
+  </si>
+  <si>
+    <t>El sistema deberá permitirle al proveedor generar un reporte consolidado (en formato de tabla) de todos los trabajos realizados por éste, con el detalle del nro. de recibo por honorarios/factura (si hubiera), tipo de servicio, cliente, fecha, dirección, descripción corta, calificación, y monto cobrado.</t>
+  </si>
+  <si>
+    <t>El sistema deberá permitirle al suministrador generar un reporte (en formato de tabla) con las ofertas, promociones y descuentos más vendidos.</t>
   </si>
 </sst>
 </file>
@@ -2266,7 +2266,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
@@ -3985,7 +3985,7 @@
   <dimension ref="B1:I58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B51" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51:D57"/>
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4923,7 +4923,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B54" s="31">
         <v>53</v>
       </c>
@@ -4931,7 +4931,7 @@
         <v>102</v>
       </c>
       <c r="D54" s="44" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>68</v>
@@ -4982,7 +4982,7 @@
         <v>323</v>
       </c>
       <c r="D57" s="44" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>68</v>
@@ -5401,10 +5401,10 @@
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C21" s="36" t="s">
+        <v>423</v>
+      </c>
+      <c r="D21" s="37" t="s">
         <v>424</v>
-      </c>
-      <c r="D21" s="37" t="s">
-        <v>425</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Reportes: Demanda de Productos y Demanda Servicios Generales
</commit_message>
<xml_diff>
--- a/Documentación/Análisis/Lista de Requerimientos - Historias de Usuarios.xlsx
+++ b/Documentación/Análisis/Lista de Requerimientos - Historias de Usuarios.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="18840" windowHeight="7725" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="18840" windowHeight="7725" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Control de versiones" sheetId="8" r:id="rId1"/>
@@ -1758,6 +1758,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1775,9 +1778,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2119,13 +2119,13 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="15"/>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="40"/>
       <c r="G3" s="16"/>
       <c r="H3" s="12"/>
     </row>
@@ -2281,7 +2281,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+    <sheetView topLeftCell="A58" workbookViewId="0">
       <selection activeCell="I59" sqref="I59"/>
     </sheetView>
   </sheetViews>
@@ -4026,8 +4026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I59"/>
   <sheetViews>
-    <sheetView topLeftCell="B55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58:F59"/>
+    <sheetView tabSelected="1" topLeftCell="B54" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4921,7 +4921,7 @@
       <c r="C51" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="D51" s="43" t="s">
+      <c r="D51" s="22" t="s">
         <v>334</v>
       </c>
       <c r="E51" s="2" t="s">
@@ -4938,7 +4938,7 @@
       <c r="C52" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="D52" s="43" t="s">
+      <c r="D52" s="22" t="s">
         <v>425</v>
       </c>
       <c r="E52" s="2" t="s">
@@ -4972,7 +4972,7 @@
       <c r="C54" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D54" s="43" t="s">
+      <c r="D54" s="22" t="s">
         <v>426</v>
       </c>
       <c r="E54" s="2" t="s">
@@ -4989,7 +4989,7 @@
       <c r="C55" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="D55" s="43" t="s">
+      <c r="D55" s="22" t="s">
         <v>335</v>
       </c>
       <c r="E55" s="2" t="s">
@@ -5006,7 +5006,7 @@
       <c r="C56" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="D56" s="43" t="s">
+      <c r="D56" s="37" t="s">
         <v>332</v>
       </c>
       <c r="E56" s="2" t="s">
@@ -5023,7 +5023,7 @@
       <c r="C57" s="7" t="s">
         <v>323</v>
       </c>
-      <c r="D57" s="43" t="s">
+      <c r="D57" s="37" t="s">
         <v>424</v>
       </c>
       <c r="E57" s="2" t="s">
@@ -5341,10 +5341,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="42" t="s">
         <v>397</v>
       </c>
-      <c r="E3" s="42"/>
+      <c r="E3" s="43"/>
     </row>
     <row r="4" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D4" s="1">
@@ -5371,10 +5371,10 @@
       </c>
     </row>
     <row r="9" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D9" s="41" t="s">
+      <c r="D9" s="42" t="s">
         <v>398</v>
       </c>
-      <c r="E9" s="42"/>
+      <c r="E9" s="43"/>
     </row>
     <row r="10" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D10" s="1">
@@ -5401,10 +5401,10 @@
       </c>
     </row>
     <row r="15" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D15" s="40" t="s">
+      <c r="D15" s="41" t="s">
         <v>399</v>
       </c>
-      <c r="E15" s="40"/>
+      <c r="E15" s="41"/>
     </row>
     <row r="16" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D16" s="1" t="s">

</xml_diff>

<commit_message>
Reporte: Proveedores destacados 80%
</commit_message>
<xml_diff>
--- a/Documentación/Análisis/Lista de Requerimientos - Historias de Usuarios.xlsx
+++ b/Documentación/Análisis/Lista de Requerimientos - Historias de Usuarios.xlsx
@@ -1111,9 +1111,6 @@
     <t>Mensaje de notificación en pantalla de bienvenida de proveedor</t>
   </si>
   <si>
-    <t>El sistema deberá permitirle al administrador generar un reporte (en formato de tabla) de los proveedores más destacados (mayor puntaje, número de trabajos, número de búsquedas, leads consumidos), para un rango de fechas dadas.</t>
-  </si>
-  <si>
     <t>Versión 3</t>
   </si>
   <si>
@@ -1415,6 +1412,9 @@
   </si>
   <si>
     <t>Así poder visualizar cuantos de los leads adquiridos por los suministradores se convierten en recargas y compras</t>
+  </si>
+  <si>
+    <t>El sistema deberá permitirle al administrador generar un reporte (en formato de tabla) de los proveedores más destacados (mayor puntaje, cantidad de trabajos, nro. de recomendaciones, nro. de volvería a contratarlo,  leads por compras), para un rango de fechas dadas.</t>
   </si>
 </sst>
 </file>
@@ -2201,7 +2201,7 @@
         <v>3</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F7" s="19" t="s">
         <v>109</v>
@@ -2301,7 +2301,7 @@
   <sheetData>
     <row r="1" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="30" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -2342,7 +2342,7 @@
         <v>114</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>119</v>
@@ -2371,7 +2371,7 @@
         <v>114</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>118</v>
@@ -2400,7 +2400,7 @@
         <v>114</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G4" s="24" t="s">
         <v>317</v>
@@ -2432,7 +2432,7 @@
         <v>313</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="H5" s="25">
         <v>3</v>
@@ -2487,7 +2487,7 @@
         <v>114</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>315</v>
@@ -2635,7 +2635,7 @@
         <v>138</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="H12" s="25">
         <v>3</v>
@@ -3003,16 +3003,16 @@
         <v>293</v>
       </c>
       <c r="D25" s="33" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E25" s="28" t="s">
         <v>308</v>
       </c>
       <c r="F25" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="G25" s="5" t="s">
         <v>383</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>384</v>
       </c>
       <c r="H25" s="25">
         <v>3</v>
@@ -3090,16 +3090,16 @@
         <v>270</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E28" s="28" t="s">
         <v>115</v>
       </c>
       <c r="F28" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="G28" s="5" t="s">
         <v>412</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>413</v>
       </c>
       <c r="H28" s="25">
         <v>2</v>
@@ -3119,16 +3119,16 @@
         <v>271</v>
       </c>
       <c r="D29" s="33" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E29" s="28" t="s">
         <v>115</v>
       </c>
       <c r="F29" s="5" t="s">
+        <v>414</v>
+      </c>
+      <c r="G29" s="5" t="s">
         <v>415</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>416</v>
       </c>
       <c r="H29" s="25">
         <v>2</v>
@@ -3148,16 +3148,16 @@
         <v>272</v>
       </c>
       <c r="D30" s="33" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E30" s="28" t="s">
         <v>115</v>
       </c>
       <c r="F30" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="G30" s="5" t="s">
         <v>417</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>418</v>
       </c>
       <c r="H30" s="25">
         <v>2</v>
@@ -3273,7 +3273,7 @@
         <v>216</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H34" s="25">
         <v>2</v>
@@ -3409,16 +3409,16 @@
         <v>322</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E39" s="28" t="s">
         <v>308</v>
       </c>
       <c r="F39" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="G39" s="5" t="s">
         <v>338</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>339</v>
       </c>
       <c r="H39" s="25">
         <v>2</v>
@@ -3589,7 +3589,7 @@
         <v>10</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>150</v>
@@ -3699,7 +3699,7 @@
         <v>273</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E49" s="28" t="s">
         <v>115</v>
@@ -3940,7 +3940,7 @@
         <v>220</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="H57" s="25">
         <v>1</v>
@@ -3955,19 +3955,19 @@
     <row r="58" spans="2:10" ht="75" x14ac:dyDescent="0.25">
       <c r="B58" s="31"/>
       <c r="C58" s="25" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E58" s="28" t="s">
         <v>308</v>
       </c>
       <c r="F58" s="5" t="s">
+        <v>431</v>
+      </c>
+      <c r="G58" s="5" t="s">
         <v>432</v>
-      </c>
-      <c r="G58" s="5" t="s">
-        <v>433</v>
       </c>
       <c r="H58" s="25">
         <v>1</v>
@@ -3976,7 +3976,7 @@
         <v>2</v>
       </c>
       <c r="J58" s="7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="59" spans="2:10" ht="45" x14ac:dyDescent="0.25">
@@ -3984,7 +3984,7 @@
         <v>57</v>
       </c>
       <c r="C59" s="25" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D59" s="5" t="s">
         <v>238</v>
@@ -4005,7 +4005,7 @@
         <v>3</v>
       </c>
       <c r="J59" s="7" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
   </sheetData>
@@ -4027,7 +4027,7 @@
   <dimension ref="B1:I59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B54" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4045,7 +4045,7 @@
   <sheetData>
     <row r="1" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="30" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
@@ -4116,7 +4116,7 @@
         <v>19</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>45</v>
@@ -4174,7 +4174,7 @@
         <v>22</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>45</v>
@@ -4310,7 +4310,7 @@
         <v>30</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>41</v>
@@ -4412,7 +4412,7 @@
         <v>36</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>41</v>
@@ -4429,7 +4429,7 @@
         <v>37</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>41</v>
@@ -4514,7 +4514,7 @@
         <v>75</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>42</v>
@@ -4531,7 +4531,7 @@
         <v>76</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>42</v>
@@ -4548,7 +4548,7 @@
         <v>77</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>42</v>
@@ -4667,7 +4667,7 @@
         <v>84</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>43</v>
@@ -4888,7 +4888,7 @@
         <v>97</v>
       </c>
       <c r="D49" s="22" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>43</v>
@@ -4905,7 +4905,7 @@
         <v>98</v>
       </c>
       <c r="D50" s="22" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>43</v>
@@ -4922,7 +4922,7 @@
         <v>99</v>
       </c>
       <c r="D51" s="22" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>68</v>
@@ -4939,7 +4939,7 @@
         <v>100</v>
       </c>
       <c r="D52" s="22" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>68</v>
@@ -4956,7 +4956,7 @@
         <v>101</v>
       </c>
       <c r="D53" s="22" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>68</v>
@@ -4973,7 +4973,7 @@
         <v>102</v>
       </c>
       <c r="D54" s="22" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>68</v>
@@ -4990,7 +4990,7 @@
         <v>111</v>
       </c>
       <c r="D55" s="22" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>68</v>
@@ -4999,7 +4999,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B56" s="31">
         <v>55</v>
       </c>
@@ -5007,7 +5007,7 @@
         <v>112</v>
       </c>
       <c r="D56" s="37" t="s">
-        <v>332</v>
+        <v>433</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>68</v>
@@ -5023,8 +5023,8 @@
       <c r="C57" s="7" t="s">
         <v>323</v>
       </c>
-      <c r="D57" s="37" t="s">
-        <v>424</v>
+      <c r="D57" s="22" t="s">
+        <v>423</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>68</v>
@@ -5036,10 +5036,10 @@
     <row r="58" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B58" s="31"/>
       <c r="C58" s="7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D58" s="22" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>68</v>
@@ -5053,7 +5053,7 @@
         <v>57</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D59" s="22" t="s">
         <v>236</v>
@@ -5103,10 +5103,10 @@
     </row>
     <row r="2" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C2" s="7" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>12</v>
@@ -5114,10 +5114,10 @@
     </row>
     <row r="3" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C3" s="7" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>12</v>
@@ -5125,10 +5125,10 @@
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C4" s="7" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>12</v>
@@ -5136,10 +5136,10 @@
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C5" s="7" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>13</v>
@@ -5147,10 +5147,10 @@
     </row>
     <row r="6" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C6" s="7" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>12</v>
@@ -5158,10 +5158,10 @@
     </row>
     <row r="7" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C7" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>13</v>
@@ -5169,10 +5169,10 @@
     </row>
     <row r="8" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C8" s="7" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>13</v>
@@ -5180,10 +5180,10 @@
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C9" s="7" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>13</v>
@@ -5191,10 +5191,10 @@
     </row>
     <row r="10" spans="3:5" ht="60" x14ac:dyDescent="0.25">
       <c r="C10" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>13</v>
@@ -5202,10 +5202,10 @@
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C11" s="7" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>13</v>
@@ -5213,10 +5213,10 @@
     </row>
     <row r="12" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C12" s="7" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>12</v>
@@ -5224,10 +5224,10 @@
     </row>
     <row r="13" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C13" s="7" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>13</v>
@@ -5235,10 +5235,10 @@
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C14" s="7" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>13</v>
@@ -5246,10 +5246,10 @@
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C15" s="7" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>12</v>
@@ -5257,10 +5257,10 @@
     </row>
     <row r="16" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C16" s="7" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>13</v>
@@ -5268,10 +5268,10 @@
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C17" s="7" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>13</v>
@@ -5279,10 +5279,10 @@
     </row>
     <row r="18" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C18" s="7" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>13</v>
@@ -5290,10 +5290,10 @@
     </row>
     <row r="19" spans="3:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C19" s="7" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>13</v>
@@ -5301,10 +5301,10 @@
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C20" s="7" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>13</v>
@@ -5312,10 +5312,10 @@
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C21" s="7" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D21" s="36" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>13</v>
@@ -5342,7 +5342,7 @@
   <sheetData>
     <row r="3" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D3" s="42" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E3" s="43"/>
     </row>
@@ -5372,7 +5372,7 @@
     </row>
     <row r="9" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D9" s="42" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E9" s="43"/>
     </row>
@@ -5402,7 +5402,7 @@
     </row>
     <row r="15" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D15" s="41" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E15" s="41"/>
     </row>
@@ -5424,10 +5424,10 @@
     </row>
     <row r="19" spans="4:8" x14ac:dyDescent="0.25">
       <c r="G19" s="32" t="s">
+        <v>399</v>
+      </c>
+      <c r="H19" s="32" t="s">
         <v>400</v>
-      </c>
-      <c r="H19" s="32" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="20" spans="4:8" ht="43.5" x14ac:dyDescent="0.25">
@@ -5435,7 +5435,7 @@
         <v>114</v>
       </c>
       <c r="H20" s="34" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="21" spans="4:8" ht="42.75" x14ac:dyDescent="0.25">
@@ -5443,7 +5443,7 @@
         <v>10</v>
       </c>
       <c r="H21" s="35" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="22" spans="4:8" ht="57.75" x14ac:dyDescent="0.25">
@@ -5451,7 +5451,7 @@
         <v>115</v>
       </c>
       <c r="H22" s="34" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="23" spans="4:8" ht="57.75" x14ac:dyDescent="0.25">
@@ -5459,7 +5459,7 @@
         <v>308</v>
       </c>
       <c r="H23" s="34" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reporte: Proveedores destacados + Recompensas 100%
</commit_message>
<xml_diff>
--- a/Documentación/Análisis/Lista de Requerimientos - Historias de Usuarios.xlsx
+++ b/Documentación/Análisis/Lista de Requerimientos - Historias de Usuarios.xlsx
@@ -1491,7 +1491,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1513,12 +1513,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1650,7 +1644,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1758,9 +1752,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2119,13 +2110,13 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="15"/>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="40"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="39"/>
       <c r="G3" s="16"/>
       <c r="H3" s="12"/>
     </row>
@@ -5006,7 +4997,7 @@
       <c r="C56" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="D56" s="37" t="s">
+      <c r="D56" s="22" t="s">
         <v>433</v>
       </c>
       <c r="E56" s="2" t="s">
@@ -5341,10 +5332,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="41" t="s">
         <v>396</v>
       </c>
-      <c r="E3" s="43"/>
+      <c r="E3" s="42"/>
     </row>
     <row r="4" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D4" s="1">
@@ -5371,10 +5362,10 @@
       </c>
     </row>
     <row r="9" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D9" s="42" t="s">
+      <c r="D9" s="41" t="s">
         <v>397</v>
       </c>
-      <c r="E9" s="43"/>
+      <c r="E9" s="42"/>
     </row>
     <row r="10" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D10" s="1">
@@ -5401,10 +5392,10 @@
       </c>
     </row>
     <row r="15" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D15" s="41" t="s">
+      <c r="D15" s="40" t="s">
         <v>398</v>
       </c>
-      <c r="E15" s="41"/>
+      <c r="E15" s="40"/>
     </row>
     <row r="16" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D16" s="1" t="s">

</xml_diff>